<commit_message>
Se agregó formato y fecha en CI1
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/Cronograma Equipo 01.xlsx
+++ b/Planificación del proyecto/Cronograma Equipo 01.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Licenciatura en Sistemas\3º AÑO\2º Cuatrimestre\Proyecto de Software\TP cuatrimesatral\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB8368B-FAD4-460B-B539-67CF4E268B22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12780" windowHeight="6075" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="1" r:id="rId1"/>
     <sheet name="CI1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -652,13 +653,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="167" formatCode="d/mm/yyyy"/>
-    <numFmt numFmtId="172" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -876,7 +875,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -887,7 +886,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -897,12 +896,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,29 +915,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -955,30 +931,55 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1193,7 +1194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1209,21 +1210,21 @@
     <col min="4" max="4" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="42" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1260,17 +1261,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="43"/>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="2">
         <f t="shared" ref="G2:H2" si="0">H2-7</f>
         <v>44067</v>
@@ -1315,7 +1316,7 @@
         <v>44137</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1342,7 +1343,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1369,7 +1370,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1382,7 +1383,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="8"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="34" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="8"/>
@@ -1394,7 +1395,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1409,7 +1410,7 @@
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="34" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="8"/>
@@ -1421,7 +1422,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1436,7 +1437,7 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="47"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="10" t="s">
         <v>19</v>
       </c>
@@ -1448,7 +1449,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8">
         <v>1.1000000000000001</v>
@@ -1466,9 +1467,9 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
@@ -1483,9 +1484,9 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
-      <c r="B10" s="43"/>
+      <c r="B10" s="30"/>
       <c r="D10" t="s">
         <v>50</v>
       </c>
@@ -1495,9 +1496,9 @@
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C11" t="s">
@@ -1512,9 +1513,9 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
-      <c r="B12" s="43"/>
+      <c r="B12" s="30"/>
       <c r="D12" t="s">
         <v>52</v>
       </c>
@@ -1524,9 +1525,9 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="30" t="s">
         <v>44</v>
       </c>
       <c r="C13" t="s">
@@ -1541,9 +1542,9 @@
       <c r="P13" s="12"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="44"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="15"/>
       <c r="D14" t="s">
         <v>54</v>
@@ -1554,9 +1555,9 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
-      <c r="B15" s="44"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="15"/>
       <c r="D15" t="s">
         <v>41</v>
@@ -1567,7 +1568,7 @@
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>48</v>
       </c>
@@ -1577,9 +1578,9 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="31" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -1594,9 +1595,9 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -1611,9 +1612,9 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" s="45"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="13"/>
       <c r="D19" s="15" t="s">
         <v>62</v>
@@ -1632,9 +1633,9 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="32" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -1657,7 +1658,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
@@ -1678,7 +1679,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
@@ -1698,7 +1699,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -1719,9 +1720,9 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="31" t="s">
         <v>65</v>
       </c>
       <c r="C24" s="15" t="s">
@@ -1744,7 +1745,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="14" t="s">
         <v>70</v>
@@ -1769,7 +1770,7 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1790,7 +1791,7 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>72</v>
@@ -1815,7 +1816,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="12"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1965,7 +1966,7 @@
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="46">
+      <c r="B45" s="33">
         <v>1.4</v>
       </c>
       <c r="C45" t="s">
@@ -2008,7 +2009,7 @@
       </c>
     </row>
     <row r="50" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="46">
+      <c r="B50" s="33">
         <v>1.5</v>
       </c>
       <c r="C50" t="s">
@@ -2051,7 +2052,7 @@
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="46">
+      <c r="B55" s="33">
         <v>1.6</v>
       </c>
       <c r="C55" t="s">
@@ -2176,14 +2177,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AK1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2195,91 +2196,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="37" t="s">
+      <c r="L1" s="45"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="38"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="40" t="s">
+      <c r="O1" s="45"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="38"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="37" t="s">
+      <c r="R1" s="45"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="38"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="40" t="s">
+      <c r="U1" s="45"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="37" t="s">
+      <c r="X1" s="45"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="40" t="s">
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="37" t="s">
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="40" t="s">
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="39"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="46"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
       <c r="K2" s="17">
         <v>44081</v>
       </c>
@@ -2362,20 +2363,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
       <c r="K3" s="23" t="s">
         <v>36</v>
       </c>
@@ -2459,29 +2460,29 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B4" s="46">
+      <c r="B4" s="33">
         <v>1.6</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="H4" s="61">
+      <c r="H4" s="40">
         <v>44081</v>
       </c>
-      <c r="I4" s="61">
-        <f t="shared" ref="I4" si="0">H4+7</f>
+      <c r="I4" s="40">
+        <f t="shared" ref="H4:I6" si="0">H4+7</f>
         <v>44088</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="41" t="s">
         <v>199</v>
       </c>
       <c r="L4" s="25"/>
@@ -2512,16 +2513,17 @@
       <c r="AK4" s="25"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="H5" s="58"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
       <c r="M5" s="25"/>
@@ -2551,19 +2553,23 @@
       <c r="AK5" s="25"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="57"/>
+      <c r="H6" s="57">
+        <v>44082</v>
+      </c>
+      <c r="I6" s="62">
+        <v>44082</v>
+      </c>
       <c r="K6" s="25" t="s">
         <v>188</v>
       </c>
@@ -2595,17 +2601,21 @@
       <c r="AK6" s="25"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="H7" s="61"/>
-      <c r="I7" s="57"/>
+      <c r="H7" s="57">
+        <v>44082</v>
+      </c>
+      <c r="I7" s="62">
+        <v>44082</v>
+      </c>
       <c r="K7" s="25" t="s">
         <v>188</v>
       </c>
@@ -2637,21 +2647,25 @@
       <c r="AK7" s="25"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="52" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="42"/>
+      <c r="H8" s="57">
+        <v>44082</v>
+      </c>
+      <c r="I8" s="62">
+        <v>44082</v>
+      </c>
+      <c r="J8" s="29"/>
       <c r="K8" s="25" t="s">
         <v>188</v>
       </c>
@@ -2683,21 +2697,25 @@
       <c r="AK8" s="25"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="52" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="42"/>
+      <c r="H9" s="57">
+        <v>44082</v>
+      </c>
+      <c r="I9" s="62">
+        <v>44082</v>
+      </c>
+      <c r="J9" s="29"/>
       <c r="K9" s="25" t="s">
         <v>188</v>
       </c>
@@ -2729,21 +2747,25 @@
       <c r="AK9" s="25"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="52" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="42"/>
+      <c r="H10" s="57">
+        <v>44082</v>
+      </c>
+      <c r="I10" s="57">
+        <v>44082</v>
+      </c>
+      <c r="J10" s="29"/>
       <c r="K10" s="25" t="s">
         <v>188</v>
       </c>
@@ -2775,21 +2797,21 @@
       <c r="AK10" s="25"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="51" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="53" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="H11" s="60"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="52" t="s">
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="37" t="s">
         <v>156</v>
       </c>
       <c r="K11" s="25"/>
@@ -2821,22 +2843,26 @@
       <c r="AK11" s="25"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="53" t="s">
+      <c r="F12" s="29"/>
+      <c r="G12" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="42"/>
+      <c r="H12" s="57">
+        <v>44083</v>
+      </c>
+      <c r="I12" s="57">
+        <v>44083</v>
+      </c>
+      <c r="J12" s="29"/>
       <c r="K12" s="25" t="s">
         <v>190</v>
       </c>
@@ -2868,20 +2894,24 @@
       <c r="AK12" s="25"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
-      <c r="D13" s="51" t="s">
+      <c r="A13" s="29"/>
+      <c r="D13" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="51" t="s">
+      <c r="F13" s="29"/>
+      <c r="G13" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="42"/>
+      <c r="H13" s="57">
+        <v>44083</v>
+      </c>
+      <c r="I13" s="57">
+        <v>44083</v>
+      </c>
+      <c r="J13" s="29"/>
       <c r="K13" s="25" t="s">
         <v>188</v>
       </c>
@@ -2913,22 +2943,26 @@
       <c r="AK13" s="25"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="52" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="52" t="s">
+      <c r="F14" s="29"/>
+      <c r="G14" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="42"/>
+      <c r="H14" s="57">
+        <v>44083</v>
+      </c>
+      <c r="I14" s="57">
+        <v>44083</v>
+      </c>
+      <c r="J14" s="29"/>
       <c r="K14" s="25" t="s">
         <v>188</v>
       </c>
@@ -2960,22 +2994,26 @@
       <c r="AK14" s="25"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="52" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="52" t="s">
+      <c r="F15" s="29"/>
+      <c r="G15" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="42"/>
+      <c r="H15" s="57">
+        <v>44083</v>
+      </c>
+      <c r="I15" s="57">
+        <v>44083</v>
+      </c>
+      <c r="J15" s="29"/>
       <c r="K15" s="25" t="s">
         <v>188</v>
       </c>
@@ -3007,22 +3045,26 @@
       <c r="AK15" s="25"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="52" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="52" t="s">
+      <c r="F16" s="29"/>
+      <c r="G16" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="57">
+        <v>44083</v>
+      </c>
+      <c r="I16" s="57">
+        <v>44083</v>
+      </c>
+      <c r="J16" s="29"/>
       <c r="K16" s="25" t="s">
         <v>188</v>
       </c>
@@ -3054,21 +3096,21 @@
       <c r="AK16" s="25"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="51" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="52" t="s">
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="52" t="s">
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="37" t="s">
         <v>156</v>
       </c>
       <c r="K17" s="25"/>
@@ -3100,22 +3142,26 @@
       <c r="AK17" s="25"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="53" t="s">
+      <c r="F18" s="29"/>
+      <c r="G18" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="57">
+        <v>44084</v>
+      </c>
+      <c r="I18" s="57">
+        <v>44084</v>
+      </c>
+      <c r="J18" s="29"/>
       <c r="K18" s="25" t="s">
         <v>190</v>
       </c>
@@ -3147,20 +3193,24 @@
       <c r="AK18" s="25"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
-      <c r="D19" s="51" t="s">
+      <c r="A19" s="29"/>
+      <c r="D19" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="51" t="s">
+      <c r="F19" s="29"/>
+      <c r="G19" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="57">
+        <v>44084</v>
+      </c>
+      <c r="I19" s="57">
+        <v>44084</v>
+      </c>
+      <c r="J19" s="29"/>
       <c r="K19" s="25" t="s">
         <v>188</v>
       </c>
@@ -3192,22 +3242,26 @@
       <c r="AK19" s="25"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="52" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="52" t="s">
+      <c r="F20" s="29"/>
+      <c r="G20" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="H20" s="57">
+        <v>44084</v>
+      </c>
+      <c r="I20" s="57">
+        <v>44084</v>
+      </c>
+      <c r="J20" s="29"/>
       <c r="K20" s="25" t="s">
         <v>188</v>
       </c>
@@ -3239,22 +3293,26 @@
       <c r="AK20" s="25"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="52" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="52" t="s">
+      <c r="F21" s="29"/>
+      <c r="G21" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
+      <c r="H21" s="57">
+        <v>44084</v>
+      </c>
+      <c r="I21" s="57">
+        <v>44084</v>
+      </c>
+      <c r="J21" s="29"/>
       <c r="K21" s="25" t="s">
         <v>188</v>
       </c>
@@ -3286,22 +3344,26 @@
       <c r="AK21" s="25"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="52" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="E22" s="53" t="s">
+      <c r="E22" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="52" t="s">
+      <c r="F22" s="29"/>
+      <c r="G22" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
+      <c r="H22" s="57">
+        <v>44084</v>
+      </c>
+      <c r="I22" s="57">
+        <v>44084</v>
+      </c>
+      <c r="J22" s="29"/>
       <c r="K22" s="25" t="s">
         <v>188</v>
       </c>
@@ -3333,21 +3395,21 @@
       <c r="AK22" s="25"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="51" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="52" t="s">
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -3377,22 +3439,26 @@
       <c r="AK23" s="25"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="53" t="s">
+      <c r="F24" s="29"/>
+      <c r="G24" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="42"/>
+      <c r="H24" s="57">
+        <v>44085</v>
+      </c>
+      <c r="I24" s="57">
+        <v>44085</v>
+      </c>
+      <c r="J24" s="29"/>
       <c r="K24" s="25" t="s">
         <v>190</v>
       </c>
@@ -3424,15 +3490,21 @@
       <c r="AK24" s="25"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D25" s="51" t="s">
+      <c r="D25" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="51" t="s">
+      <c r="F25" s="29"/>
+      <c r="G25" s="36" t="s">
         <v>188</v>
+      </c>
+      <c r="H25" s="57">
+        <v>44085</v>
+      </c>
+      <c r="I25" s="57">
+        <v>44085</v>
       </c>
       <c r="K25" s="25" t="s">
         <v>188</v>
@@ -3465,17 +3537,23 @@
       <c r="AK25" s="25"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B26" s="48"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="52" t="s">
+      <c r="B26" s="35"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="52" t="s">
+      <c r="F26" s="29"/>
+      <c r="G26" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H26" s="57">
+        <v>44085</v>
+      </c>
+      <c r="I26" s="57">
+        <v>44085</v>
       </c>
       <c r="K26" s="25" t="s">
         <v>188</v>
@@ -3508,17 +3586,23 @@
       <c r="AK26" s="25"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B27" s="48"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="52" t="s">
+      <c r="B27" s="35"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="E27" s="52" t="s">
+      <c r="E27" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="52" t="s">
+      <c r="F27" s="29"/>
+      <c r="G27" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H27" s="57">
+        <v>44085</v>
+      </c>
+      <c r="I27" s="57">
+        <v>44085</v>
       </c>
       <c r="K27" s="25" t="s">
         <v>188</v>
@@ -3551,17 +3635,23 @@
       <c r="AK27" s="25"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B28" s="48"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="52" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E28" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="F28" s="42"/>
-      <c r="G28" s="52" t="s">
+      <c r="F28" s="29"/>
+      <c r="G28" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H28" s="57">
+        <v>44085</v>
+      </c>
+      <c r="I28" s="57">
+        <v>44085</v>
       </c>
       <c r="K28" s="25" t="s">
         <v>188</v>
@@ -3594,17 +3684,23 @@
       <c r="AK28" s="25"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B29" s="48"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="52" t="s">
+      <c r="B29" s="35"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="52" t="s">
+      <c r="F29" s="29"/>
+      <c r="G29" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H29" s="57">
+        <v>44085</v>
+      </c>
+      <c r="I29" s="57">
+        <v>44085</v>
       </c>
       <c r="K29" s="25" t="s">
         <v>188</v>
@@ -3637,18 +3733,20 @@
       <c r="AK29" s="25"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="52" t="s">
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="J30" s="51" t="s">
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="36" t="s">
         <v>162</v>
       </c>
       <c r="K30" s="25"/>
@@ -3680,17 +3778,23 @@
       <c r="AK30" s="25"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51" t="s">
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="F31" s="42"/>
-      <c r="G31" s="53" t="s">
+      <c r="F31" s="29"/>
+      <c r="G31" s="38" t="s">
         <v>190</v>
+      </c>
+      <c r="H31" s="57">
+        <v>44086</v>
+      </c>
+      <c r="I31" s="57">
+        <v>44086</v>
       </c>
       <c r="K31" s="25" t="s">
         <v>190</v>
@@ -3723,14 +3827,20 @@
       <c r="AK31" s="25"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D32" s="51" t="s">
+      <c r="D32" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="G32" s="51" t="s">
+      <c r="G32" s="36" t="s">
         <v>188</v>
+      </c>
+      <c r="H32" s="57">
+        <v>44086</v>
+      </c>
+      <c r="I32" s="57">
+        <v>44086</v>
       </c>
       <c r="K32" s="25" t="s">
         <v>188</v>
@@ -3763,16 +3873,22 @@
       <c r="AK32" s="25"/>
     </row>
     <row r="33" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B33" s="48"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="52" t="s">
+      <c r="B33" s="35"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="E33" s="51" t="s">
+      <c r="E33" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="G33" s="52" t="s">
+      <c r="G33" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H33" s="57">
+        <v>44086</v>
+      </c>
+      <c r="I33" s="57">
+        <v>44086</v>
       </c>
       <c r="K33" s="25" t="s">
         <v>188</v>
@@ -3805,16 +3921,22 @@
       <c r="AK33" s="25"/>
     </row>
     <row r="34" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B34" s="48"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="52" t="s">
+      <c r="B34" s="35"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="G34" s="52" t="s">
+      <c r="G34" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H34" s="57">
+        <v>44086</v>
+      </c>
+      <c r="I34" s="57">
+        <v>44086</v>
       </c>
       <c r="K34" s="25" t="s">
         <v>188</v>
@@ -3847,16 +3969,22 @@
       <c r="AK34" s="25"/>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B35" s="48"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="52" t="s">
+      <c r="B35" s="35"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="G35" s="52" t="s">
+      <c r="G35" s="37" t="s">
         <v>188</v>
+      </c>
+      <c r="H35" s="57">
+        <v>44086</v>
+      </c>
+      <c r="I35" s="57">
+        <v>44086</v>
       </c>
       <c r="K35" s="25" t="s">
         <v>188</v>
@@ -3889,12 +4017,14 @@
       <c r="AK35" s="25"/>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B36" s="46">
+      <c r="B36" s="33">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="36" t="s">
         <v>40</v>
       </c>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
       <c r="K36" s="25"/>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -3924,6 +4054,9 @@
       <c r="AK36" s="25"/>
     </row>
     <row r="37" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="D37" s="36"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
       <c r="K37" s="25"/>
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
@@ -3953,18 +4086,20 @@
       <c r="AK37" s="25"/>
     </row>
     <row r="38" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="51" t="s">
+      <c r="C38" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="G38" s="51" t="s">
+      <c r="G38" s="36" t="s">
         <v>200</v>
       </c>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
       <c r="K38" s="25"/>
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
@@ -3994,14 +4129,20 @@
       <c r="AK38" s="25"/>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="D39" s="51" t="s">
+      <c r="D39" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="E39" s="51" t="s">
+      <c r="E39" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="G39" s="51" t="s">
+      <c r="G39" s="36" t="s">
         <v>193</v>
+      </c>
+      <c r="H39" s="57">
+        <v>44087</v>
+      </c>
+      <c r="I39" s="57">
+        <v>44087</v>
       </c>
       <c r="K39" s="25" t="s">
         <v>193</v>
@@ -4034,14 +4175,20 @@
       <c r="AK39" s="25"/>
     </row>
     <row r="40" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="D40" s="51" t="s">
+      <c r="D40" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="E40" s="51" t="s">
+      <c r="E40" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="G40" s="51" t="s">
+      <c r="G40" s="36" t="s">
         <v>193</v>
+      </c>
+      <c r="H40" s="57">
+        <v>44087</v>
+      </c>
+      <c r="I40" s="57">
+        <v>44087</v>
       </c>
       <c r="K40" s="25" t="s">
         <v>193</v>
@@ -32118,6 +32265,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -32126,17 +32283,8 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Establecidas las fechas para entregables - Semana 1
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/Cronograma Equipo 01.xlsx
+++ b/Planificación del proyecto/Cronograma Equipo 01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="1" r:id="rId1"/>
@@ -997,29 +997,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1042,6 +1019,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1264,8 +1264,8 @@
   </sheetPr>
   <dimension ref="A1:AA88"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1275,20 +1275,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="49" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1326,16 +1326,16 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="2">
         <f t="shared" ref="G2:H2" si="0">H2-7</f>
         <v>44067</v>
@@ -1381,15 +1381,15 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="55">
+      <c r="A3" s="42">
         <v>1</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="36">
@@ -1408,27 +1408,27 @@
       <c r="O3" s="37"/>
       <c r="P3" s="37"/>
       <c r="Q3" s="37"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="45"/>
+      <c r="X3" s="45"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="45"/>
+      <c r="AA3" s="45"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="55">
+      <c r="A4" s="42">
         <v>2</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="57" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="36">
@@ -1447,27 +1447,27 @@
       <c r="O4" s="37"/>
       <c r="P4" s="37"/>
       <c r="Q4" s="37"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="45"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="55">
+      <c r="A5" s="42">
         <v>3</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="57" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="36"/>
@@ -1484,27 +1484,27 @@
       <c r="O5" s="37"/>
       <c r="P5" s="37"/>
       <c r="Q5" s="37"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="58"/>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="58"/>
-      <c r="Y5" s="58"/>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="45"/>
+      <c r="X5" s="45"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="45"/>
+      <c r="AA5" s="45"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55">
+      <c r="A6" s="42">
         <v>4</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="57" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="38">
@@ -1523,27 +1523,27 @@
       <c r="O6" s="37"/>
       <c r="P6" s="37"/>
       <c r="Q6" s="37"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="45"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="55">
+      <c r="A7" s="42">
         <v>5</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="57" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="38">
@@ -1562,31 +1562,31 @@
       <c r="O7" s="37"/>
       <c r="P7" s="37"/>
       <c r="Q7" s="37"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="58"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="45"/>
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="55">
+      <c r="A8" s="42">
         <v>6</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="45">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="22">
@@ -1605,31 +1605,31 @@
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="58"/>
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="58"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="45"/>
+      <c r="AA8" s="45"/>
     </row>
     <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="55">
+      <c r="A9" s="42">
         <v>7</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="35">
@@ -1648,27 +1648,27 @@
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
       <c r="Q9" s="37"/>
-      <c r="R9" s="58"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="58"/>
-      <c r="U9" s="58"/>
-      <c r="V9" s="58"/>
-      <c r="W9" s="58"/>
-      <c r="X9" s="58"/>
-      <c r="Y9" s="58"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="58"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="45"/>
+      <c r="U9" s="45"/>
+      <c r="V9" s="45"/>
+      <c r="W9" s="45"/>
+      <c r="X9" s="45"/>
+      <c r="Y9" s="45"/>
+      <c r="Z9" s="45"/>
+      <c r="AA9" s="45"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="55">
+      <c r="A10" s="42">
         <v>8</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="21" t="s">
@@ -1687,31 +1687,31 @@
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
       <c r="Q10" s="37"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="58"/>
-      <c r="Y10" s="58"/>
-      <c r="Z10" s="58"/>
-      <c r="AA10" s="58"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="45"/>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="45"/>
+      <c r="X10" s="45"/>
+      <c r="Y10" s="45"/>
+      <c r="Z10" s="45"/>
+      <c r="AA10" s="45"/>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="55">
+      <c r="A11" s="42">
         <v>9</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="22">
@@ -1730,27 +1730,27 @@
       <c r="O11" s="37"/>
       <c r="P11" s="37"/>
       <c r="Q11" s="37"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
-      <c r="T11" s="58"/>
-      <c r="U11" s="58"/>
-      <c r="V11" s="58"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="58"/>
-      <c r="Y11" s="58"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="58"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="45"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="55">
+      <c r="A12" s="42">
         <v>10</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58" t="s">
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="21" t="s">
@@ -1769,31 +1769,31 @@
       <c r="O12" s="37"/>
       <c r="P12" s="37"/>
       <c r="Q12" s="37"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="58"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="45"/>
+      <c r="AA12" s="45"/>
     </row>
     <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="55">
+      <c r="A13" s="42">
         <v>11</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="22">
@@ -1812,27 +1812,27 @@
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
       <c r="Q13" s="37"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="58"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="45"/>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="45"/>
     </row>
     <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="55">
+      <c r="A14" s="42">
         <v>12</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="58" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="22">
@@ -1852,27 +1852,27 @@
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
-      <c r="V14" s="58"/>
-      <c r="W14" s="58"/>
-      <c r="X14" s="58"/>
-      <c r="Y14" s="58"/>
-      <c r="Z14" s="58"/>
-      <c r="AA14" s="58"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="45"/>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="55">
+      <c r="A15" s="42">
         <v>13</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="58" t="s">
+      <c r="B15" s="46"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="25">
@@ -1891,27 +1891,27 @@
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
       <c r="Q15" s="37"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58"/>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="58"/>
-      <c r="Z15" s="58"/>
-      <c r="AA15" s="58"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+      <c r="X15" s="45"/>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="45"/>
     </row>
     <row r="16" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="55">
+      <c r="A16" s="42">
         <v>14</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58" t="s">
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="25">
@@ -1930,31 +1930,31 @@
       <c r="O16" s="37"/>
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
-      <c r="R16" s="58"/>
-      <c r="S16" s="58"/>
-      <c r="T16" s="58"/>
-      <c r="U16" s="58"/>
-      <c r="V16" s="58"/>
-      <c r="W16" s="58"/>
-      <c r="X16" s="58"/>
-      <c r="Y16" s="58"/>
-      <c r="Z16" s="58"/>
-      <c r="AA16" s="58"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="45"/>
     </row>
     <row r="17" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="55">
+      <c r="A17" s="42">
         <v>15</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="40">
@@ -1973,31 +1973,31 @@
       <c r="O17" s="37"/>
       <c r="P17" s="37"/>
       <c r="Q17" s="37"/>
-      <c r="R17" s="58"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="58"/>
-      <c r="Y17" s="58"/>
-      <c r="Z17" s="58"/>
-      <c r="AA17" s="58"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
+      <c r="AA17" s="45"/>
     </row>
     <row r="18" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="55">
+      <c r="A18" s="42">
         <v>16</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D18" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="57" t="s">
+      <c r="E18" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="40">
@@ -2016,27 +2016,27 @@
       <c r="O18" s="37"/>
       <c r="P18" s="37"/>
       <c r="Q18" s="37"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="58"/>
-      <c r="AA18" s="58"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="45"/>
     </row>
     <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="55">
+      <c r="A19" s="42">
         <v>17</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="24">
@@ -2055,31 +2055,31 @@
       </c>
       <c r="P19" s="37"/>
       <c r="Q19" s="37"/>
-      <c r="R19" s="58"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="58"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="58"/>
-      <c r="Z19" s="58"/>
-      <c r="AA19" s="58"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="45"/>
     </row>
     <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="55">
+      <c r="A20" s="42">
         <v>18</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="40">
@@ -2098,27 +2098,27 @@
         <v>208</v>
       </c>
       <c r="Q20" s="37"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="58"/>
-      <c r="X20" s="58"/>
-      <c r="Y20" s="58"/>
-      <c r="Z20" s="58"/>
-      <c r="AA20" s="58"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
+      <c r="W20" s="45"/>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="45"/>
     </row>
     <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="55">
+      <c r="A21" s="42">
         <v>19</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55" t="s">
+      <c r="B21" s="46"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="40">
@@ -2137,27 +2137,27 @@
       <c r="Q21" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="58"/>
-      <c r="Y21" s="58"/>
-      <c r="Z21" s="58"/>
-      <c r="AA21" s="58"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="45"/>
+      <c r="W21" s="45"/>
+      <c r="X21" s="45"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="45"/>
+      <c r="AA21" s="45"/>
     </row>
     <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="55">
+      <c r="A22" s="42">
         <v>20</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55" t="s">
+      <c r="B22" s="45"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="24">
@@ -2176,27 +2176,27 @@
       <c r="Q22" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="58"/>
-      <c r="Y22" s="58"/>
-      <c r="Z22" s="58"/>
-      <c r="AA22" s="58"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="45"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="45"/>
     </row>
     <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="55">
+      <c r="A23" s="42">
         <v>21</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="58" t="s">
+      <c r="B23" s="46"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="24">
@@ -2215,31 +2215,31 @@
       <c r="Q23" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="R23" s="58"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="58"/>
-      <c r="AA23" s="58"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="45"/>
     </row>
     <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="55">
+      <c r="A24" s="42">
         <v>22</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="24">
@@ -2258,31 +2258,31 @@
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
       <c r="Q24" s="37"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="58"/>
-      <c r="W24" s="58"/>
-      <c r="X24" s="58"/>
-      <c r="Y24" s="58"/>
-      <c r="Z24" s="58"/>
-      <c r="AA24" s="58"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="45"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="45"/>
+      <c r="Z24" s="45"/>
+      <c r="AA24" s="45"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="55">
+      <c r="A25" s="42">
         <v>23</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="57" t="s">
+      <c r="E25" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F25" s="40">
@@ -2301,27 +2301,27 @@
       <c r="O25" s="37"/>
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="58"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="45"/>
+      <c r="W25" s="45"/>
+      <c r="X25" s="45"/>
+      <c r="Y25" s="45"/>
+      <c r="Z25" s="45"/>
+      <c r="AA25" s="45"/>
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="55">
+      <c r="A26" s="42">
         <v>24</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55" t="s">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="57" t="s">
+      <c r="E26" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="40">
@@ -2340,34 +2340,34 @@
       <c r="O26" s="37"/>
       <c r="P26" s="37"/>
       <c r="Q26" s="37"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="58"/>
-      <c r="Y26" s="58"/>
-      <c r="Z26" s="58"/>
-      <c r="AA26" s="58"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="45"/>
+      <c r="V26" s="45"/>
+      <c r="W26" s="45"/>
+      <c r="X26" s="45"/>
+      <c r="Y26" s="45"/>
+      <c r="Z26" s="45"/>
+      <c r="AA26" s="45"/>
     </row>
     <row r="27" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="55">
+      <c r="A27" s="42">
         <v>25</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="41">
         <v>44094</v>
       </c>
       <c r="G27" s="37"/>
@@ -2383,27 +2383,27 @@
       <c r="O27" s="37"/>
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="58"/>
-      <c r="V27" s="58"/>
-      <c r="W27" s="58"/>
-      <c r="X27" s="58"/>
-      <c r="Y27" s="58"/>
-      <c r="Z27" s="58"/>
-      <c r="AA27" s="58"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
+      <c r="U27" s="45"/>
+      <c r="V27" s="45"/>
+      <c r="W27" s="45"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="45"/>
+      <c r="Z27" s="45"/>
+      <c r="AA27" s="45"/>
     </row>
     <row r="28" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="55">
+      <c r="A28" s="42">
         <v>26</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55" t="s">
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F28" s="40" t="s">
@@ -2422,34 +2422,34 @@
       <c r="O28" s="37"/>
       <c r="P28" s="37"/>
       <c r="Q28" s="37"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
-      <c r="V28" s="58"/>
-      <c r="W28" s="58"/>
-      <c r="X28" s="58"/>
-      <c r="Y28" s="58"/>
-      <c r="Z28" s="58"/>
-      <c r="AA28" s="58"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="45"/>
+      <c r="W28" s="45"/>
+      <c r="X28" s="45"/>
+      <c r="Y28" s="45"/>
+      <c r="Z28" s="45"/>
+      <c r="AA28" s="45"/>
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="55">
+      <c r="A29" s="42">
         <v>27</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="54">
+      <c r="F29" s="41">
         <v>44094</v>
       </c>
       <c r="G29" s="39"/>
@@ -2465,27 +2465,27 @@
       <c r="O29" s="39"/>
       <c r="P29" s="39"/>
       <c r="Q29" s="39"/>
-      <c r="R29" s="58"/>
-      <c r="S29" s="58"/>
-      <c r="T29" s="58"/>
-      <c r="U29" s="58"/>
-      <c r="V29" s="58"/>
-      <c r="W29" s="58"/>
-      <c r="X29" s="58"/>
-      <c r="Y29" s="58"/>
-      <c r="Z29" s="58"/>
-      <c r="AA29" s="58"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="45"/>
+      <c r="AA29" s="45"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55">
+      <c r="A30" s="42">
         <v>28</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="55" t="s">
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F30" s="40" t="s">
@@ -2504,34 +2504,34 @@
       <c r="O30" s="39"/>
       <c r="P30" s="39"/>
       <c r="Q30" s="39"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="58"/>
-      <c r="V30" s="58"/>
-      <c r="W30" s="58"/>
-      <c r="X30" s="58"/>
-      <c r="Y30" s="58"/>
-      <c r="Z30" s="58"/>
-      <c r="AA30" s="58"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
+      <c r="X30" s="45"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="45"/>
+      <c r="AA30" s="45"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="55">
+      <c r="A31" s="42">
         <v>29</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="55" t="s">
+      <c r="D31" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="54">
+      <c r="F31" s="41">
         <v>44094</v>
       </c>
       <c r="G31" s="39"/>
@@ -2547,27 +2547,27 @@
       <c r="O31" s="39"/>
       <c r="P31" s="39"/>
       <c r="Q31" s="39"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
-      <c r="U31" s="58"/>
-      <c r="V31" s="58"/>
-      <c r="W31" s="58"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="58"/>
-      <c r="Z31" s="58"/>
-      <c r="AA31" s="58"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="X31" s="45"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="45"/>
+      <c r="AA31" s="45"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="55">
+      <c r="A32" s="42">
         <v>30</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="55" t="s">
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="40" t="s">
@@ -2586,31 +2586,31 @@
       <c r="O32" s="39"/>
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
-      <c r="T32" s="58"/>
-      <c r="U32" s="58"/>
-      <c r="V32" s="58"/>
-      <c r="W32" s="58"/>
-      <c r="X32" s="58"/>
-      <c r="Y32" s="58"/>
-      <c r="Z32" s="58"/>
-      <c r="AA32" s="58"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="45"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="55">
+      <c r="A33" s="42">
         <v>31</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="55" t="s">
+      <c r="D33" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="57" t="s">
+      <c r="E33" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F33" s="40">
@@ -2629,27 +2629,27 @@
       <c r="O33" s="39"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
-      <c r="T33" s="58"/>
-      <c r="U33" s="58"/>
-      <c r="V33" s="58"/>
-      <c r="W33" s="58"/>
-      <c r="X33" s="58"/>
-      <c r="Y33" s="58"/>
-      <c r="Z33" s="58"/>
-      <c r="AA33" s="58"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="45"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="55">
+      <c r="A34" s="42">
         <v>32</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="55" t="s">
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="57" t="s">
+      <c r="E34" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F34" s="40">
@@ -2668,31 +2668,31 @@
       <c r="O34" s="39"/>
       <c r="P34" s="39"/>
       <c r="Q34" s="39"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="58"/>
-      <c r="V34" s="58"/>
-      <c r="W34" s="58"/>
-      <c r="X34" s="58"/>
-      <c r="Y34" s="58"/>
-      <c r="Z34" s="58"/>
-      <c r="AA34" s="58"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="55">
+      <c r="A35" s="42">
         <v>33</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="58" t="s">
+      <c r="C35" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="57" t="s">
+      <c r="E35" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="40">
@@ -2711,27 +2711,27 @@
       <c r="O35" s="39"/>
       <c r="P35" s="39"/>
       <c r="Q35" s="39"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="58"/>
-      <c r="T35" s="58"/>
-      <c r="U35" s="58"/>
-      <c r="V35" s="58"/>
-      <c r="W35" s="58"/>
-      <c r="X35" s="58"/>
-      <c r="Y35" s="58"/>
-      <c r="Z35" s="58"/>
-      <c r="AA35" s="58"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="45"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="45"/>
+      <c r="W35" s="45"/>
+      <c r="X35" s="45"/>
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="45"/>
+      <c r="AA35" s="45"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="55">
+      <c r="A36" s="42">
         <v>34</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="55" t="s">
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="57" t="s">
+      <c r="E36" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F36" s="40">
@@ -2750,31 +2750,31 @@
       <c r="O36" s="39"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="58"/>
-      <c r="T36" s="58"/>
-      <c r="U36" s="58"/>
-      <c r="V36" s="58"/>
-      <c r="W36" s="58"/>
-      <c r="X36" s="58"/>
-      <c r="Y36" s="58"/>
-      <c r="Z36" s="58"/>
-      <c r="AA36" s="58"/>
+      <c r="R36" s="45"/>
+      <c r="S36" s="45"/>
+      <c r="T36" s="45"/>
+      <c r="U36" s="45"/>
+      <c r="V36" s="45"/>
+      <c r="W36" s="45"/>
+      <c r="X36" s="45"/>
+      <c r="Y36" s="45"/>
+      <c r="Z36" s="45"/>
+      <c r="AA36" s="45"/>
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="55">
+      <c r="A37" s="42">
         <v>35</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="58" t="s">
+      <c r="D37" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="57" t="s">
+      <c r="E37" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="40">
@@ -2793,30 +2793,30 @@
       <c r="O37" s="39"/>
       <c r="P37" s="39"/>
       <c r="Q37" s="39"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="58"/>
-      <c r="W37" s="58"/>
-      <c r="X37" s="58"/>
-      <c r="Y37" s="58"/>
-      <c r="Z37" s="58"/>
-      <c r="AA37" s="58"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="45"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="55">
+      <c r="A38" s="42">
         <v>36</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58" t="s">
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="E38" s="57" t="s">
+      <c r="E38" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="54">
+      <c r="F38" s="41">
         <v>44094</v>
       </c>
       <c r="G38" s="39"/>
@@ -2832,34 +2832,34 @@
       <c r="O38" s="39"/>
       <c r="P38" s="39"/>
       <c r="Q38" s="39"/>
-      <c r="R38" s="58"/>
-      <c r="S38" s="58"/>
-      <c r="T38" s="58"/>
-      <c r="U38" s="58"/>
-      <c r="V38" s="58"/>
-      <c r="W38" s="58"/>
-      <c r="X38" s="58"/>
-      <c r="Y38" s="58"/>
-      <c r="Z38" s="58"/>
-      <c r="AA38" s="58"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="45"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="45"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="55">
+      <c r="A39" s="42">
         <v>37</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="58" t="s">
+      <c r="C39" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="57" t="s">
+      <c r="E39" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="54">
+      <c r="F39" s="41">
         <v>44094</v>
       </c>
       <c r="G39" s="39"/>
@@ -2875,27 +2875,27 @@
       <c r="O39" s="39"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
-      <c r="R39" s="58"/>
-      <c r="S39" s="58"/>
-      <c r="T39" s="58"/>
-      <c r="U39" s="58"/>
-      <c r="V39" s="58"/>
-      <c r="W39" s="58"/>
-      <c r="X39" s="58"/>
-      <c r="Y39" s="58"/>
-      <c r="Z39" s="58"/>
-      <c r="AA39" s="58"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="45"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="55">
+      <c r="A40" s="42">
         <v>38</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58" t="s">
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="57" t="s">
+      <c r="E40" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F40" s="40">
@@ -2914,31 +2914,31 @@
       <c r="O40" s="39"/>
       <c r="P40" s="39"/>
       <c r="Q40" s="39"/>
-      <c r="R40" s="58"/>
-      <c r="S40" s="58"/>
-      <c r="T40" s="58"/>
-      <c r="U40" s="58"/>
-      <c r="V40" s="58"/>
-      <c r="W40" s="58"/>
-      <c r="X40" s="58"/>
-      <c r="Y40" s="58"/>
-      <c r="Z40" s="58"/>
-      <c r="AA40" s="58"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="55">
+      <c r="A41" s="42">
         <v>39</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="58" t="s">
+      <c r="C41" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="57" t="s">
+      <c r="E41" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="40">
@@ -2957,27 +2957,27 @@
       <c r="O41" s="39"/>
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
-      <c r="R41" s="58"/>
-      <c r="S41" s="58"/>
-      <c r="T41" s="58"/>
-      <c r="U41" s="58"/>
-      <c r="V41" s="58"/>
-      <c r="W41" s="58"/>
-      <c r="X41" s="58"/>
-      <c r="Y41" s="58"/>
-      <c r="Z41" s="58"/>
-      <c r="AA41" s="58"/>
+      <c r="R41" s="45"/>
+      <c r="S41" s="45"/>
+      <c r="T41" s="45"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="45"/>
+      <c r="X41" s="45"/>
+      <c r="Y41" s="45"/>
+      <c r="Z41" s="45"/>
+      <c r="AA41" s="45"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="55">
+      <c r="A42" s="42">
         <v>40</v>
       </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58" t="s">
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="57" t="s">
+      <c r="E42" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F42" s="40">
@@ -2996,31 +2996,31 @@
       <c r="O42" s="39"/>
       <c r="P42" s="39"/>
       <c r="Q42" s="39"/>
-      <c r="R42" s="58"/>
-      <c r="S42" s="58"/>
-      <c r="T42" s="58"/>
-      <c r="U42" s="58"/>
-      <c r="V42" s="58"/>
-      <c r="W42" s="58"/>
-      <c r="X42" s="58"/>
-      <c r="Y42" s="58"/>
-      <c r="Z42" s="58"/>
-      <c r="AA42" s="58"/>
+      <c r="R42" s="45"/>
+      <c r="S42" s="45"/>
+      <c r="T42" s="45"/>
+      <c r="U42" s="45"/>
+      <c r="V42" s="45"/>
+      <c r="W42" s="45"/>
+      <c r="X42" s="45"/>
+      <c r="Y42" s="45"/>
+      <c r="Z42" s="45"/>
+      <c r="AA42" s="45"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="55">
+      <c r="A43" s="42">
         <v>41</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D43" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="57" t="s">
+      <c r="E43" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="40">
@@ -3039,27 +3039,27 @@
       <c r="O43" s="39"/>
       <c r="P43" s="39"/>
       <c r="Q43" s="39"/>
-      <c r="R43" s="58"/>
-      <c r="S43" s="58"/>
-      <c r="T43" s="58"/>
-      <c r="U43" s="58"/>
-      <c r="V43" s="58"/>
-      <c r="W43" s="58"/>
-      <c r="X43" s="58"/>
-      <c r="Y43" s="58"/>
-      <c r="Z43" s="58"/>
-      <c r="AA43" s="58"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="45"/>
+      <c r="T43" s="45"/>
+      <c r="U43" s="45"/>
+      <c r="V43" s="45"/>
+      <c r="W43" s="45"/>
+      <c r="X43" s="45"/>
+      <c r="Y43" s="45"/>
+      <c r="Z43" s="45"/>
+      <c r="AA43" s="45"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="55">
+      <c r="A44" s="42">
         <v>42</v>
       </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58" t="s">
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E44" s="57" t="s">
+      <c r="E44" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F44" s="40">
@@ -3078,27 +3078,27 @@
       <c r="O44" s="39"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="39"/>
-      <c r="R44" s="58"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="58"/>
-      <c r="U44" s="58"/>
-      <c r="V44" s="58"/>
-      <c r="W44" s="58"/>
-      <c r="X44" s="58"/>
-      <c r="Y44" s="58"/>
-      <c r="Z44" s="58"/>
-      <c r="AA44" s="58"/>
+      <c r="R44" s="45"/>
+      <c r="S44" s="45"/>
+      <c r="T44" s="45"/>
+      <c r="U44" s="45"/>
+      <c r="V44" s="45"/>
+      <c r="W44" s="45"/>
+      <c r="X44" s="45"/>
+      <c r="Y44" s="45"/>
+      <c r="Z44" s="45"/>
+      <c r="AA44" s="45"/>
     </row>
     <row r="45" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="55">
+      <c r="A45" s="42">
         <v>43</v>
       </c>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58" t="s">
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="E45" s="57" t="s">
+      <c r="E45" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="40">
@@ -3117,27 +3117,27 @@
       <c r="O45" s="39"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
-      <c r="R45" s="58"/>
-      <c r="S45" s="58"/>
-      <c r="T45" s="58"/>
-      <c r="U45" s="58"/>
-      <c r="V45" s="58"/>
-      <c r="W45" s="58"/>
-      <c r="X45" s="58"/>
-      <c r="Y45" s="58"/>
-      <c r="Z45" s="58"/>
-      <c r="AA45" s="58"/>
+      <c r="R45" s="45"/>
+      <c r="S45" s="45"/>
+      <c r="T45" s="45"/>
+      <c r="U45" s="45"/>
+      <c r="V45" s="45"/>
+      <c r="W45" s="45"/>
+      <c r="X45" s="45"/>
+      <c r="Y45" s="45"/>
+      <c r="Z45" s="45"/>
+      <c r="AA45" s="45"/>
     </row>
     <row r="46" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="55">
+      <c r="A46" s="42">
         <v>44</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58" t="s">
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E46" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F46" s="40">
@@ -3156,31 +3156,31 @@
       <c r="O46" s="39"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
-      <c r="R46" s="58"/>
-      <c r="S46" s="58"/>
-      <c r="T46" s="58"/>
-      <c r="U46" s="58"/>
-      <c r="V46" s="58"/>
-      <c r="W46" s="58"/>
-      <c r="X46" s="58"/>
-      <c r="Y46" s="58"/>
-      <c r="Z46" s="58"/>
-      <c r="AA46" s="58"/>
+      <c r="R46" s="45"/>
+      <c r="S46" s="45"/>
+      <c r="T46" s="45"/>
+      <c r="U46" s="45"/>
+      <c r="V46" s="45"/>
+      <c r="W46" s="45"/>
+      <c r="X46" s="45"/>
+      <c r="Y46" s="45"/>
+      <c r="Z46" s="45"/>
+      <c r="AA46" s="45"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="55">
+      <c r="A47" s="42">
         <v>45</v>
       </c>
-      <c r="B47" s="58">
+      <c r="B47" s="45">
         <v>1.4</v>
       </c>
-      <c r="C47" s="58" t="s">
+      <c r="C47" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="58" t="s">
+      <c r="D47" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F47" s="24">
@@ -3199,31 +3199,31 @@
       <c r="O47" s="39"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="39"/>
-      <c r="R47" s="58"/>
-      <c r="S47" s="58"/>
-      <c r="T47" s="58"/>
-      <c r="U47" s="58"/>
-      <c r="V47" s="58"/>
-      <c r="W47" s="58"/>
-      <c r="X47" s="58"/>
-      <c r="Y47" s="58"/>
-      <c r="Z47" s="58"/>
-      <c r="AA47" s="58"/>
+      <c r="R47" s="45"/>
+      <c r="S47" s="45"/>
+      <c r="T47" s="45"/>
+      <c r="U47" s="45"/>
+      <c r="V47" s="45"/>
+      <c r="W47" s="45"/>
+      <c r="X47" s="45"/>
+      <c r="Y47" s="45"/>
+      <c r="Z47" s="45"/>
+      <c r="AA47" s="45"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="55">
+      <c r="A48" s="42">
         <v>46</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="58" t="s">
+      <c r="C48" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="58" t="s">
+      <c r="D48" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="E48" s="57" t="s">
+      <c r="E48" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F48" s="40">
@@ -3242,30 +3242,30 @@
       <c r="O48" s="39"/>
       <c r="P48" s="39"/>
       <c r="Q48" s="39"/>
-      <c r="R48" s="58"/>
-      <c r="S48" s="58"/>
-      <c r="T48" s="58"/>
-      <c r="U48" s="58"/>
-      <c r="V48" s="58"/>
-      <c r="W48" s="58"/>
-      <c r="X48" s="58"/>
-      <c r="Y48" s="58"/>
-      <c r="Z48" s="58"/>
-      <c r="AA48" s="58"/>
+      <c r="R48" s="45"/>
+      <c r="S48" s="45"/>
+      <c r="T48" s="45"/>
+      <c r="U48" s="45"/>
+      <c r="V48" s="45"/>
+      <c r="W48" s="45"/>
+      <c r="X48" s="45"/>
+      <c r="Y48" s="45"/>
+      <c r="Z48" s="45"/>
+      <c r="AA48" s="45"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="55">
+      <c r="A49" s="42">
         <v>47</v>
       </c>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58" t="s">
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="57" t="s">
+      <c r="E49" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="54">
+      <c r="F49" s="41">
         <v>44101</v>
       </c>
       <c r="G49" s="39"/>
@@ -3281,34 +3281,34 @@
       <c r="O49" s="39"/>
       <c r="P49" s="39"/>
       <c r="Q49" s="39"/>
-      <c r="R49" s="58"/>
-      <c r="S49" s="58"/>
-      <c r="T49" s="58"/>
-      <c r="U49" s="58"/>
-      <c r="V49" s="58"/>
-      <c r="W49" s="58"/>
-      <c r="X49" s="58"/>
-      <c r="Y49" s="58"/>
-      <c r="Z49" s="58"/>
-      <c r="AA49" s="58"/>
+      <c r="R49" s="45"/>
+      <c r="S49" s="45"/>
+      <c r="T49" s="45"/>
+      <c r="U49" s="45"/>
+      <c r="V49" s="45"/>
+      <c r="W49" s="45"/>
+      <c r="X49" s="45"/>
+      <c r="Y49" s="45"/>
+      <c r="Z49" s="45"/>
+      <c r="AA49" s="45"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="55">
+      <c r="A50" s="42">
         <v>48</v>
       </c>
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="58" t="s">
+      <c r="C50" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="58" t="s">
+      <c r="D50" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F50" s="54">
+      <c r="F50" s="41">
         <v>44129</v>
       </c>
       <c r="G50" s="39"/>
@@ -3319,32 +3319,32 @@
       <c r="L50" s="39"/>
       <c r="M50" s="39"/>
       <c r="N50" s="39"/>
-      <c r="O50" s="58"/>
+      <c r="O50" s="45"/>
       <c r="P50" s="39" t="s">
         <v>208</v>
       </c>
       <c r="Q50" s="39"/>
-      <c r="R50" s="58"/>
-      <c r="S50" s="58"/>
-      <c r="T50" s="58"/>
-      <c r="U50" s="58"/>
-      <c r="V50" s="58"/>
-      <c r="W50" s="58"/>
-      <c r="X50" s="58"/>
-      <c r="Y50" s="58"/>
-      <c r="Z50" s="58"/>
-      <c r="AA50" s="58"/>
+      <c r="R50" s="45"/>
+      <c r="S50" s="45"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="45"/>
+      <c r="V50" s="45"/>
+      <c r="W50" s="45"/>
+      <c r="X50" s="45"/>
+      <c r="Y50" s="45"/>
+      <c r="Z50" s="45"/>
+      <c r="AA50" s="45"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="55">
+      <c r="A51" s="42">
         <v>49</v>
       </c>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58" t="s">
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="E51" s="57" t="s">
+      <c r="E51" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F51" s="25">
@@ -3359,31 +3359,31 @@
       <c r="M51" s="39"/>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
-      <c r="P51" s="58"/>
+      <c r="P51" s="45"/>
       <c r="Q51" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="R51" s="58"/>
-      <c r="S51" s="58"/>
-      <c r="T51" s="58"/>
-      <c r="U51" s="58"/>
-      <c r="V51" s="58"/>
-      <c r="W51" s="58"/>
-      <c r="X51" s="58"/>
-      <c r="Y51" s="58"/>
-      <c r="Z51" s="58"/>
-      <c r="AA51" s="58"/>
+      <c r="R51" s="45"/>
+      <c r="S51" s="45"/>
+      <c r="T51" s="45"/>
+      <c r="U51" s="45"/>
+      <c r="V51" s="45"/>
+      <c r="W51" s="45"/>
+      <c r="X51" s="45"/>
+      <c r="Y51" s="45"/>
+      <c r="Z51" s="45"/>
+      <c r="AA51" s="45"/>
     </row>
     <row r="52" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="55">
+      <c r="A52" s="42">
         <v>50</v>
       </c>
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58" t="s">
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E52" s="57" t="s">
+      <c r="E52" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F52" s="25">
@@ -3402,27 +3402,27 @@
       <c r="Q52" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R52" s="58"/>
-      <c r="S52" s="58"/>
-      <c r="T52" s="58"/>
-      <c r="U52" s="58"/>
-      <c r="V52" s="58"/>
-      <c r="W52" s="58"/>
-      <c r="X52" s="58"/>
-      <c r="Y52" s="58"/>
-      <c r="Z52" s="58"/>
-      <c r="AA52" s="58"/>
+      <c r="R52" s="45"/>
+      <c r="S52" s="45"/>
+      <c r="T52" s="45"/>
+      <c r="U52" s="45"/>
+      <c r="V52" s="45"/>
+      <c r="W52" s="45"/>
+      <c r="X52" s="45"/>
+      <c r="Y52" s="45"/>
+      <c r="Z52" s="45"/>
+      <c r="AA52" s="45"/>
     </row>
     <row r="53" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="55">
+      <c r="A53" s="42">
         <v>51</v>
       </c>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58" t="s">
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="E53" s="57" t="s">
+      <c r="E53" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F53" s="25">
@@ -3441,31 +3441,31 @@
       <c r="Q53" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R53" s="58"/>
-      <c r="S53" s="58"/>
-      <c r="T53" s="58"/>
-      <c r="U53" s="58"/>
-      <c r="V53" s="58"/>
-      <c r="W53" s="58"/>
-      <c r="X53" s="58"/>
-      <c r="Y53" s="58"/>
-      <c r="Z53" s="58"/>
-      <c r="AA53" s="58"/>
+      <c r="R53" s="45"/>
+      <c r="S53" s="45"/>
+      <c r="T53" s="45"/>
+      <c r="U53" s="45"/>
+      <c r="V53" s="45"/>
+      <c r="W53" s="45"/>
+      <c r="X53" s="45"/>
+      <c r="Y53" s="45"/>
+      <c r="Z53" s="45"/>
+      <c r="AA53" s="45"/>
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="55">
+      <c r="A54" s="42">
         <v>52</v>
       </c>
-      <c r="B54" s="58">
+      <c r="B54" s="45">
         <v>1.5</v>
       </c>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="58" t="s">
+      <c r="D54" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="E54" s="57" t="s">
+      <c r="E54" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F54" s="25">
@@ -3484,34 +3484,34 @@
       <c r="O54" s="39"/>
       <c r="P54" s="39"/>
       <c r="Q54" s="39"/>
-      <c r="R54" s="58"/>
-      <c r="S54" s="58"/>
-      <c r="T54" s="58"/>
-      <c r="U54" s="58"/>
-      <c r="V54" s="58"/>
-      <c r="W54" s="58"/>
-      <c r="X54" s="58"/>
-      <c r="Y54" s="58"/>
-      <c r="Z54" s="58"/>
-      <c r="AA54" s="58"/>
+      <c r="R54" s="45"/>
+      <c r="S54" s="45"/>
+      <c r="T54" s="45"/>
+      <c r="U54" s="45"/>
+      <c r="V54" s="45"/>
+      <c r="W54" s="45"/>
+      <c r="X54" s="45"/>
+      <c r="Y54" s="45"/>
+      <c r="Z54" s="45"/>
+      <c r="AA54" s="45"/>
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="55">
+      <c r="A55" s="42">
         <v>53</v>
       </c>
-      <c r="B55" s="58" t="s">
+      <c r="B55" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="58" t="s">
+      <c r="C55" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="E55" s="57" t="s">
+      <c r="E55" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F55" s="54">
+      <c r="F55" s="41">
         <v>44122</v>
       </c>
       <c r="G55" s="39"/>
@@ -3527,27 +3527,27 @@
       </c>
       <c r="P55" s="39"/>
       <c r="Q55" s="39"/>
-      <c r="R55" s="58"/>
-      <c r="S55" s="58"/>
-      <c r="T55" s="58"/>
-      <c r="U55" s="58"/>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="58"/>
-      <c r="Y55" s="58"/>
-      <c r="Z55" s="58"/>
-      <c r="AA55" s="58"/>
+      <c r="R55" s="45"/>
+      <c r="S55" s="45"/>
+      <c r="T55" s="45"/>
+      <c r="U55" s="45"/>
+      <c r="V55" s="45"/>
+      <c r="W55" s="45"/>
+      <c r="X55" s="45"/>
+      <c r="Y55" s="45"/>
+      <c r="Z55" s="45"/>
+      <c r="AA55" s="45"/>
     </row>
     <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="55">
+      <c r="A56" s="42">
         <v>54</v>
       </c>
-      <c r="B56" s="58"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58" t="s">
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="E56" s="57" t="s">
+      <c r="E56" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F56" s="25">
@@ -3566,34 +3566,34 @@
         <v>19</v>
       </c>
       <c r="Q56" s="39"/>
-      <c r="R56" s="58"/>
-      <c r="S56" s="58"/>
-      <c r="T56" s="58"/>
-      <c r="U56" s="58"/>
-      <c r="V56" s="58"/>
-      <c r="W56" s="58"/>
-      <c r="X56" s="58"/>
-      <c r="Y56" s="58"/>
-      <c r="Z56" s="58"/>
-      <c r="AA56" s="58"/>
+      <c r="R56" s="45"/>
+      <c r="S56" s="45"/>
+      <c r="T56" s="45"/>
+      <c r="U56" s="45"/>
+      <c r="V56" s="45"/>
+      <c r="W56" s="45"/>
+      <c r="X56" s="45"/>
+      <c r="Y56" s="45"/>
+      <c r="Z56" s="45"/>
+      <c r="AA56" s="45"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="55">
+      <c r="A57" s="42">
         <v>55</v>
       </c>
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="C57" s="58" t="s">
+      <c r="C57" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="D57" s="58" t="s">
+      <c r="D57" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="E57" s="57" t="s">
+      <c r="E57" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F57" s="54">
+      <c r="F57" s="41">
         <v>44129</v>
       </c>
       <c r="G57" s="39"/>
@@ -3609,30 +3609,30 @@
         <v>19</v>
       </c>
       <c r="Q57" s="39"/>
-      <c r="R57" s="58"/>
-      <c r="S57" s="58"/>
-      <c r="T57" s="58"/>
-      <c r="U57" s="58"/>
-      <c r="V57" s="58"/>
-      <c r="W57" s="58"/>
-      <c r="X57" s="58"/>
-      <c r="Y57" s="58"/>
-      <c r="Z57" s="58"/>
-      <c r="AA57" s="58"/>
+      <c r="R57" s="45"/>
+      <c r="S57" s="45"/>
+      <c r="T57" s="45"/>
+      <c r="U57" s="45"/>
+      <c r="V57" s="45"/>
+      <c r="W57" s="45"/>
+      <c r="X57" s="45"/>
+      <c r="Y57" s="45"/>
+      <c r="Z57" s="45"/>
+      <c r="AA57" s="45"/>
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="55">
+      <c r="A58" s="42">
         <v>56</v>
       </c>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58" t="s">
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="E58" s="57" t="s">
+      <c r="E58" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F58" s="54">
+      <c r="F58" s="41">
         <v>44136</v>
       </c>
       <c r="G58" s="39"/>
@@ -3648,30 +3648,30 @@
       <c r="Q58" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R58" s="58"/>
-      <c r="S58" s="58"/>
-      <c r="T58" s="58"/>
-      <c r="U58" s="58"/>
-      <c r="V58" s="58"/>
-      <c r="W58" s="58"/>
-      <c r="X58" s="58"/>
-      <c r="Y58" s="58"/>
-      <c r="Z58" s="58"/>
-      <c r="AA58" s="58"/>
+      <c r="R58" s="45"/>
+      <c r="S58" s="45"/>
+      <c r="T58" s="45"/>
+      <c r="U58" s="45"/>
+      <c r="V58" s="45"/>
+      <c r="W58" s="45"/>
+      <c r="X58" s="45"/>
+      <c r="Y58" s="45"/>
+      <c r="Z58" s="45"/>
+      <c r="AA58" s="45"/>
     </row>
     <row r="59" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="55">
+      <c r="A59" s="42">
         <v>57</v>
       </c>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58" t="s">
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="E59" s="57" t="s">
+      <c r="E59" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F59" s="54">
+      <c r="F59" s="41">
         <v>44136</v>
       </c>
       <c r="G59" s="39"/>
@@ -3687,30 +3687,30 @@
       <c r="Q59" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R59" s="58"/>
-      <c r="S59" s="58"/>
-      <c r="T59" s="58"/>
-      <c r="U59" s="58"/>
-      <c r="V59" s="58"/>
-      <c r="W59" s="58"/>
-      <c r="X59" s="58"/>
-      <c r="Y59" s="58"/>
-      <c r="Z59" s="58"/>
-      <c r="AA59" s="58"/>
+      <c r="R59" s="45"/>
+      <c r="S59" s="45"/>
+      <c r="T59" s="45"/>
+      <c r="U59" s="45"/>
+      <c r="V59" s="45"/>
+      <c r="W59" s="45"/>
+      <c r="X59" s="45"/>
+      <c r="Y59" s="45"/>
+      <c r="Z59" s="45"/>
+      <c r="AA59" s="45"/>
     </row>
     <row r="60" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="55">
+      <c r="A60" s="42">
         <v>58</v>
       </c>
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58" t="s">
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="E60" s="57" t="s">
+      <c r="E60" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F60" s="54">
+      <c r="F60" s="41">
         <v>44136</v>
       </c>
       <c r="G60" s="39"/>
@@ -3726,31 +3726,31 @@
       <c r="Q60" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R60" s="58"/>
-      <c r="S60" s="58"/>
-      <c r="T60" s="58"/>
-      <c r="U60" s="58"/>
-      <c r="V60" s="58"/>
-      <c r="W60" s="58"/>
-      <c r="X60" s="58"/>
-      <c r="Y60" s="58"/>
-      <c r="Z60" s="58"/>
-      <c r="AA60" s="58"/>
+      <c r="R60" s="45"/>
+      <c r="S60" s="45"/>
+      <c r="T60" s="45"/>
+      <c r="U60" s="45"/>
+      <c r="V60" s="45"/>
+      <c r="W60" s="45"/>
+      <c r="X60" s="45"/>
+      <c r="Y60" s="45"/>
+      <c r="Z60" s="45"/>
+      <c r="AA60" s="45"/>
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="55">
+      <c r="A61" s="42">
         <v>59</v>
       </c>
-      <c r="B61" s="58">
+      <c r="B61" s="45">
         <v>1.6</v>
       </c>
-      <c r="C61" s="58" t="s">
+      <c r="C61" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="D61" s="58" t="s">
+      <c r="D61" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="E61" s="57" t="s">
+      <c r="E61" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F61" s="25">
@@ -3771,29 +3771,29 @@
       <c r="O61" s="39"/>
       <c r="P61" s="39"/>
       <c r="Q61" s="39"/>
-      <c r="R61" s="58"/>
-      <c r="S61" s="58"/>
-      <c r="T61" s="58"/>
-      <c r="U61" s="58"/>
-      <c r="V61" s="58"/>
-      <c r="W61" s="58"/>
-      <c r="X61" s="58"/>
-      <c r="Y61" s="58"/>
-      <c r="Z61" s="58"/>
-      <c r="AA61" s="58"/>
+      <c r="R61" s="45"/>
+      <c r="S61" s="45"/>
+      <c r="T61" s="45"/>
+      <c r="U61" s="45"/>
+      <c r="V61" s="45"/>
+      <c r="W61" s="45"/>
+      <c r="X61" s="45"/>
+      <c r="Y61" s="45"/>
+      <c r="Z61" s="45"/>
+      <c r="AA61" s="45"/>
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="55">
+      <c r="A62" s="42">
         <v>60</v>
       </c>
-      <c r="B62" s="58"/>
-      <c r="C62" s="58" t="s">
+      <c r="B62" s="45"/>
+      <c r="C62" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="58" t="s">
+      <c r="D62" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="E62" s="57" t="s">
+      <c r="E62" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F62" s="24">
@@ -3812,30 +3812,30 @@
       <c r="O62" s="39"/>
       <c r="P62" s="39"/>
       <c r="Q62" s="39"/>
-      <c r="R62" s="58"/>
-      <c r="S62" s="58"/>
-      <c r="T62" s="58"/>
-      <c r="U62" s="58"/>
-      <c r="V62" s="58"/>
-      <c r="W62" s="58"/>
-      <c r="X62" s="58"/>
-      <c r="Y62" s="58"/>
-      <c r="Z62" s="58"/>
-      <c r="AA62" s="58"/>
+      <c r="R62" s="45"/>
+      <c r="S62" s="45"/>
+      <c r="T62" s="45"/>
+      <c r="U62" s="45"/>
+      <c r="V62" s="45"/>
+      <c r="W62" s="45"/>
+      <c r="X62" s="45"/>
+      <c r="Y62" s="45"/>
+      <c r="Z62" s="45"/>
+      <c r="AA62" s="45"/>
     </row>
     <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="55">
+      <c r="A63" s="42">
         <v>61</v>
       </c>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58" t="s">
+      <c r="B63" s="45"/>
+      <c r="C63" s="45"/>
+      <c r="D63" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="E63" s="57" t="s">
+      <c r="E63" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="54">
+      <c r="F63" s="41">
         <v>44087</v>
       </c>
       <c r="G63" s="39"/>
@@ -3851,33 +3851,33 @@
       <c r="O63" s="39"/>
       <c r="P63" s="39"/>
       <c r="Q63" s="39"/>
-      <c r="R63" s="58"/>
-      <c r="S63" s="58"/>
-      <c r="T63" s="58"/>
-      <c r="U63" s="58"/>
-      <c r="V63" s="58"/>
-      <c r="W63" s="58"/>
-      <c r="X63" s="58"/>
-      <c r="Y63" s="58"/>
-      <c r="Z63" s="58"/>
-      <c r="AA63" s="58"/>
+      <c r="R63" s="45"/>
+      <c r="S63" s="45"/>
+      <c r="T63" s="45"/>
+      <c r="U63" s="45"/>
+      <c r="V63" s="45"/>
+      <c r="W63" s="45"/>
+      <c r="X63" s="45"/>
+      <c r="Y63" s="45"/>
+      <c r="Z63" s="45"/>
+      <c r="AA63" s="45"/>
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="55">
+      <c r="A64" s="42">
         <v>62</v>
       </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58" t="s">
+      <c r="B64" s="45"/>
+      <c r="C64" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="58" t="s">
+      <c r="D64" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="E64" s="57" t="s">
+      <c r="E64" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F64" s="24">
-        <v>44081</v>
+        <v>44082</v>
       </c>
       <c r="G64" s="39"/>
       <c r="H64" s="39"/>
@@ -3892,27 +3892,27 @@
       <c r="O64" s="39"/>
       <c r="P64" s="39"/>
       <c r="Q64" s="39"/>
-      <c r="R64" s="58"/>
-      <c r="S64" s="58"/>
-      <c r="T64" s="58"/>
-      <c r="U64" s="58"/>
-      <c r="V64" s="58"/>
-      <c r="W64" s="58"/>
-      <c r="X64" s="58"/>
-      <c r="Y64" s="58"/>
-      <c r="Z64" s="58"/>
-      <c r="AA64" s="58"/>
+      <c r="R64" s="45"/>
+      <c r="S64" s="45"/>
+      <c r="T64" s="45"/>
+      <c r="U64" s="45"/>
+      <c r="V64" s="45"/>
+      <c r="W64" s="45"/>
+      <c r="X64" s="45"/>
+      <c r="Y64" s="45"/>
+      <c r="Z64" s="45"/>
+      <c r="AA64" s="45"/>
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="55">
+      <c r="A65" s="42">
         <v>63</v>
       </c>
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58" t="s">
+      <c r="B65" s="45"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="E65" s="57" t="s">
+      <c r="E65" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F65" s="40">
@@ -3931,33 +3931,33 @@
       <c r="O65" s="39"/>
       <c r="P65" s="39"/>
       <c r="Q65" s="39"/>
-      <c r="R65" s="58"/>
-      <c r="S65" s="58"/>
-      <c r="T65" s="58"/>
-      <c r="U65" s="58"/>
-      <c r="V65" s="58"/>
-      <c r="W65" s="58"/>
-      <c r="X65" s="58"/>
-      <c r="Y65" s="58"/>
-      <c r="Z65" s="58"/>
-      <c r="AA65" s="58"/>
+      <c r="R65" s="45"/>
+      <c r="S65" s="45"/>
+      <c r="T65" s="45"/>
+      <c r="U65" s="45"/>
+      <c r="V65" s="45"/>
+      <c r="W65" s="45"/>
+      <c r="X65" s="45"/>
+      <c r="Y65" s="45"/>
+      <c r="Z65" s="45"/>
+      <c r="AA65" s="45"/>
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="55">
+      <c r="A66" s="42">
         <v>64</v>
       </c>
-      <c r="B66" s="58"/>
-      <c r="C66" s="58" t="s">
+      <c r="B66" s="45"/>
+      <c r="C66" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="D66" s="58" t="s">
+      <c r="D66" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="E66" s="57" t="s">
+      <c r="E66" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F66" s="24">
-        <v>44081</v>
+        <v>44083</v>
       </c>
       <c r="G66" s="39"/>
       <c r="H66" s="39"/>
@@ -3972,27 +3972,27 @@
       <c r="O66" s="39"/>
       <c r="P66" s="39"/>
       <c r="Q66" s="39"/>
-      <c r="R66" s="58"/>
-      <c r="S66" s="58"/>
-      <c r="T66" s="58"/>
-      <c r="U66" s="58"/>
-      <c r="V66" s="58"/>
-      <c r="W66" s="58"/>
-      <c r="X66" s="58"/>
-      <c r="Y66" s="58"/>
-      <c r="Z66" s="58"/>
-      <c r="AA66" s="58"/>
+      <c r="R66" s="45"/>
+      <c r="S66" s="45"/>
+      <c r="T66" s="45"/>
+      <c r="U66" s="45"/>
+      <c r="V66" s="45"/>
+      <c r="W66" s="45"/>
+      <c r="X66" s="45"/>
+      <c r="Y66" s="45"/>
+      <c r="Z66" s="45"/>
+      <c r="AA66" s="45"/>
     </row>
     <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="55">
+      <c r="A67" s="42">
         <v>65</v>
       </c>
-      <c r="B67" s="58"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58" t="s">
+      <c r="B67" s="45"/>
+      <c r="C67" s="45"/>
+      <c r="D67" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="E67" s="57" t="s">
+      <c r="E67" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F67" s="40">
@@ -4011,33 +4011,33 @@
       <c r="O67" s="39"/>
       <c r="P67" s="39"/>
       <c r="Q67" s="39"/>
-      <c r="R67" s="58"/>
-      <c r="S67" s="58"/>
-      <c r="T67" s="58"/>
-      <c r="U67" s="58"/>
-      <c r="V67" s="58"/>
-      <c r="W67" s="58"/>
-      <c r="X67" s="58"/>
-      <c r="Y67" s="58"/>
-      <c r="Z67" s="58"/>
-      <c r="AA67" s="58"/>
+      <c r="R67" s="45"/>
+      <c r="S67" s="45"/>
+      <c r="T67" s="45"/>
+      <c r="U67" s="45"/>
+      <c r="V67" s="45"/>
+      <c r="W67" s="45"/>
+      <c r="X67" s="45"/>
+      <c r="Y67" s="45"/>
+      <c r="Z67" s="45"/>
+      <c r="AA67" s="45"/>
     </row>
     <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="55">
+      <c r="A68" s="42">
         <v>66</v>
       </c>
-      <c r="B68" s="58"/>
-      <c r="C68" s="58" t="s">
+      <c r="B68" s="45"/>
+      <c r="C68" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="58" t="s">
+      <c r="D68" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="E68" s="57" t="s">
+      <c r="E68" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F68" s="24">
-        <v>44081</v>
+        <v>44084</v>
       </c>
       <c r="G68" s="39"/>
       <c r="H68" s="39"/>
@@ -4052,27 +4052,27 @@
       <c r="O68" s="39"/>
       <c r="P68" s="39"/>
       <c r="Q68" s="39"/>
-      <c r="R68" s="58"/>
-      <c r="S68" s="58"/>
-      <c r="T68" s="58"/>
-      <c r="U68" s="58"/>
-      <c r="V68" s="58"/>
-      <c r="W68" s="58"/>
-      <c r="X68" s="58"/>
-      <c r="Y68" s="58"/>
-      <c r="Z68" s="58"/>
-      <c r="AA68" s="58"/>
+      <c r="R68" s="45"/>
+      <c r="S68" s="45"/>
+      <c r="T68" s="45"/>
+      <c r="U68" s="45"/>
+      <c r="V68" s="45"/>
+      <c r="W68" s="45"/>
+      <c r="X68" s="45"/>
+      <c r="Y68" s="45"/>
+      <c r="Z68" s="45"/>
+      <c r="AA68" s="45"/>
     </row>
     <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="55">
+      <c r="A69" s="42">
         <v>67</v>
       </c>
-      <c r="B69" s="58"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58" t="s">
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="E69" s="57" t="s">
+      <c r="E69" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F69" s="40">
@@ -4091,31 +4091,33 @@
       <c r="O69" s="39"/>
       <c r="P69" s="39"/>
       <c r="Q69" s="39"/>
-      <c r="R69" s="58"/>
-      <c r="S69" s="58"/>
-      <c r="T69" s="58"/>
-      <c r="U69" s="58"/>
-      <c r="V69" s="58"/>
-      <c r="W69" s="58"/>
-      <c r="X69" s="58"/>
-      <c r="Y69" s="58"/>
-      <c r="Z69" s="58"/>
-      <c r="AA69" s="58"/>
+      <c r="R69" s="45"/>
+      <c r="S69" s="45"/>
+      <c r="T69" s="45"/>
+      <c r="U69" s="45"/>
+      <c r="V69" s="45"/>
+      <c r="W69" s="45"/>
+      <c r="X69" s="45"/>
+      <c r="Y69" s="45"/>
+      <c r="Z69" s="45"/>
+      <c r="AA69" s="45"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="55">
+      <c r="A70" s="42">
         <v>68</v>
       </c>
-      <c r="B70" s="58"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58" t="s">
+      <c r="B70" s="45"/>
+      <c r="C70" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="E70" s="57" t="s">
+      <c r="E70" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F70" s="24">
-        <v>44081</v>
+        <v>44085</v>
       </c>
       <c r="G70" s="39"/>
       <c r="H70" s="39"/>
@@ -4130,29 +4132,26 @@
       <c r="O70" s="39"/>
       <c r="P70" s="39"/>
       <c r="Q70" s="39"/>
-      <c r="R70" s="58"/>
-      <c r="S70" s="58"/>
-      <c r="T70" s="58"/>
-      <c r="U70" s="58"/>
-      <c r="V70" s="58"/>
-      <c r="W70" s="58"/>
-      <c r="X70" s="58"/>
-      <c r="Y70" s="58"/>
-      <c r="Z70" s="58"/>
-      <c r="AA70" s="58"/>
+      <c r="R70" s="45"/>
+      <c r="S70" s="45"/>
+      <c r="T70" s="45"/>
+      <c r="U70" s="45"/>
+      <c r="V70" s="45"/>
+      <c r="W70" s="45"/>
+      <c r="X70" s="45"/>
+      <c r="Y70" s="45"/>
+      <c r="Z70" s="45"/>
+      <c r="AA70" s="45"/>
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="55">
+      <c r="A71" s="42">
         <v>69</v>
       </c>
-      <c r="B71" s="58"/>
-      <c r="C71" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="D71" s="58" t="s">
+      <c r="B71" s="45"/>
+      <c r="D71" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="E71" s="57" t="s">
+      <c r="E71" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F71" s="40">
@@ -4171,27 +4170,27 @@
       <c r="O71" s="39"/>
       <c r="P71" s="39"/>
       <c r="Q71" s="39"/>
-      <c r="R71" s="58"/>
-      <c r="S71" s="58"/>
-      <c r="T71" s="58"/>
-      <c r="U71" s="58"/>
-      <c r="V71" s="58"/>
-      <c r="W71" s="58"/>
-      <c r="X71" s="58"/>
-      <c r="Y71" s="58"/>
-      <c r="Z71" s="58"/>
-      <c r="AA71" s="58"/>
+      <c r="R71" s="45"/>
+      <c r="S71" s="45"/>
+      <c r="T71" s="45"/>
+      <c r="U71" s="45"/>
+      <c r="V71" s="45"/>
+      <c r="W71" s="45"/>
+      <c r="X71" s="45"/>
+      <c r="Y71" s="45"/>
+      <c r="Z71" s="45"/>
+      <c r="AA71" s="45"/>
     </row>
     <row r="72" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="55">
+      <c r="A72" s="42">
         <v>70</v>
       </c>
-      <c r="B72" s="58"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58" t="s">
+      <c r="B72" s="45"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="E72" s="57" t="s">
+      <c r="E72" s="44" t="s">
         <v>21</v>
       </c>
       <c r="F72" s="35">
@@ -4210,27 +4209,27 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="39"/>
-      <c r="R72" s="58"/>
-      <c r="S72" s="58"/>
-      <c r="T72" s="58"/>
-      <c r="U72" s="58"/>
-      <c r="V72" s="58"/>
-      <c r="W72" s="58"/>
-      <c r="X72" s="58"/>
-      <c r="Y72" s="58"/>
-      <c r="Z72" s="58"/>
-      <c r="AA72" s="58"/>
+      <c r="R72" s="45"/>
+      <c r="S72" s="45"/>
+      <c r="T72" s="45"/>
+      <c r="U72" s="45"/>
+      <c r="V72" s="45"/>
+      <c r="W72" s="45"/>
+      <c r="X72" s="45"/>
+      <c r="Y72" s="45"/>
+      <c r="Z72" s="45"/>
+      <c r="AA72" s="45"/>
     </row>
     <row r="73" spans="1:27" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="55">
+      <c r="A73" s="42">
         <v>71</v>
       </c>
-      <c r="B73" s="58"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58" t="s">
+      <c r="B73" s="45"/>
+      <c r="C73" s="45"/>
+      <c r="D73" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="E73" s="57" t="s">
+      <c r="E73" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F73" s="35">
@@ -4249,495 +4248,495 @@
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
       <c r="Q73" s="39"/>
-      <c r="R73" s="58"/>
-      <c r="S73" s="58"/>
-      <c r="T73" s="58"/>
-      <c r="U73" s="58"/>
-      <c r="V73" s="58"/>
-      <c r="W73" s="58"/>
-      <c r="X73" s="58"/>
-      <c r="Y73" s="58"/>
-      <c r="Z73" s="58"/>
-      <c r="AA73" s="58"/>
+      <c r="R73" s="45"/>
+      <c r="S73" s="45"/>
+      <c r="T73" s="45"/>
+      <c r="U73" s="45"/>
+      <c r="V73" s="45"/>
+      <c r="W73" s="45"/>
+      <c r="X73" s="45"/>
+      <c r="Y73" s="45"/>
+      <c r="Z73" s="45"/>
+      <c r="AA73" s="45"/>
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="55">
+      <c r="A74" s="42">
         <v>72</v>
       </c>
-      <c r="B74" s="58">
+      <c r="B74" s="45">
         <v>1.7</v>
       </c>
-      <c r="C74" s="58" t="s">
+      <c r="C74" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="D74" s="58" t="s">
+      <c r="D74" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E74" s="57" t="s">
+      <c r="E74" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F74" s="60">
+      <c r="F74" s="47">
         <v>44067</v>
       </c>
-      <c r="G74" s="61" t="s">
+      <c r="G74" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="H74" s="61"/>
-      <c r="I74" s="61"/>
-      <c r="J74" s="61"/>
-      <c r="K74" s="61"/>
-      <c r="L74" s="61"/>
-      <c r="M74" s="61"/>
-      <c r="N74" s="61"/>
-      <c r="O74" s="61"/>
-      <c r="P74" s="61"/>
-      <c r="Q74" s="61"/>
-      <c r="R74" s="58"/>
-      <c r="S74" s="58"/>
-      <c r="T74" s="58"/>
-      <c r="U74" s="58"/>
-      <c r="V74" s="58"/>
-      <c r="W74" s="58"/>
-      <c r="X74" s="58"/>
-      <c r="Y74" s="58"/>
-      <c r="Z74" s="58"/>
-      <c r="AA74" s="58"/>
+      <c r="H74" s="48"/>
+      <c r="I74" s="48"/>
+      <c r="J74" s="48"/>
+      <c r="K74" s="48"/>
+      <c r="L74" s="48"/>
+      <c r="M74" s="48"/>
+      <c r="N74" s="48"/>
+      <c r="O74" s="48"/>
+      <c r="P74" s="48"/>
+      <c r="Q74" s="48"/>
+      <c r="R74" s="45"/>
+      <c r="S74" s="45"/>
+      <c r="T74" s="45"/>
+      <c r="U74" s="45"/>
+      <c r="V74" s="45"/>
+      <c r="W74" s="45"/>
+      <c r="X74" s="45"/>
+      <c r="Y74" s="45"/>
+      <c r="Z74" s="45"/>
+      <c r="AA74" s="45"/>
     </row>
     <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="55">
+      <c r="A75" s="42">
         <v>73</v>
       </c>
-      <c r="B75" s="58"/>
-      <c r="C75" s="58" t="s">
+      <c r="B75" s="45"/>
+      <c r="C75" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D75" s="58"/>
-      <c r="E75" s="57" t="s">
+      <c r="D75" s="45"/>
+      <c r="E75" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
-      <c r="J75" s="58"/>
-      <c r="K75" s="58"/>
-      <c r="L75" s="58"/>
-      <c r="M75" s="58"/>
-      <c r="N75" s="58"/>
-      <c r="O75" s="58"/>
-      <c r="P75" s="58"/>
-      <c r="Q75" s="58"/>
-      <c r="R75" s="58"/>
-      <c r="S75" s="58"/>
-      <c r="T75" s="58"/>
-      <c r="U75" s="58"/>
-      <c r="V75" s="58"/>
-      <c r="W75" s="58"/>
-      <c r="X75" s="58"/>
-      <c r="Y75" s="58"/>
-      <c r="Z75" s="58"/>
-      <c r="AA75" s="58"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="45"/>
+      <c r="I75" s="45"/>
+      <c r="J75" s="45"/>
+      <c r="K75" s="45"/>
+      <c r="L75" s="45"/>
+      <c r="M75" s="45"/>
+      <c r="N75" s="45"/>
+      <c r="O75" s="45"/>
+      <c r="P75" s="45"/>
+      <c r="Q75" s="45"/>
+      <c r="R75" s="45"/>
+      <c r="S75" s="45"/>
+      <c r="T75" s="45"/>
+      <c r="U75" s="45"/>
+      <c r="V75" s="45"/>
+      <c r="W75" s="45"/>
+      <c r="X75" s="45"/>
+      <c r="Y75" s="45"/>
+      <c r="Z75" s="45"/>
+      <c r="AA75" s="45"/>
     </row>
     <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="55">
+      <c r="A76" s="42">
         <v>74</v>
       </c>
-      <c r="B76" s="58"/>
-      <c r="C76" s="58" t="s">
+      <c r="B76" s="45"/>
+      <c r="C76" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="D76" s="58"/>
-      <c r="E76" s="57" t="s">
+      <c r="D76" s="45"/>
+      <c r="E76" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F76" s="58"/>
-      <c r="G76" s="58"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
-      <c r="J76" s="58"/>
-      <c r="K76" s="58"/>
-      <c r="L76" s="58"/>
-      <c r="M76" s="58"/>
-      <c r="N76" s="58"/>
-      <c r="O76" s="58"/>
-      <c r="P76" s="58"/>
-      <c r="Q76" s="58"/>
-      <c r="R76" s="58"/>
-      <c r="S76" s="58"/>
-      <c r="T76" s="58"/>
-      <c r="U76" s="58"/>
-      <c r="V76" s="58"/>
-      <c r="W76" s="58"/>
-      <c r="X76" s="58"/>
-      <c r="Y76" s="58"/>
-      <c r="Z76" s="58"/>
-      <c r="AA76" s="58"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="45"/>
+      <c r="J76" s="45"/>
+      <c r="K76" s="45"/>
+      <c r="L76" s="45"/>
+      <c r="M76" s="45"/>
+      <c r="N76" s="45"/>
+      <c r="O76" s="45"/>
+      <c r="P76" s="45"/>
+      <c r="Q76" s="45"/>
+      <c r="R76" s="45"/>
+      <c r="S76" s="45"/>
+      <c r="T76" s="45"/>
+      <c r="U76" s="45"/>
+      <c r="V76" s="45"/>
+      <c r="W76" s="45"/>
+      <c r="X76" s="45"/>
+      <c r="Y76" s="45"/>
+      <c r="Z76" s="45"/>
+      <c r="AA76" s="45"/>
     </row>
     <row r="77" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="55">
+      <c r="A77" s="42">
         <v>75</v>
       </c>
-      <c r="B77" s="58"/>
-      <c r="C77" s="58" t="s">
+      <c r="B77" s="45"/>
+      <c r="C77" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="D77" s="58"/>
-      <c r="E77" s="57" t="s">
+      <c r="D77" s="45"/>
+      <c r="E77" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F77" s="58"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="58"/>
-      <c r="I77" s="58"/>
-      <c r="J77" s="58"/>
-      <c r="K77" s="58"/>
-      <c r="L77" s="58"/>
-      <c r="M77" s="58"/>
-      <c r="N77" s="58"/>
-      <c r="O77" s="58"/>
-      <c r="P77" s="58"/>
-      <c r="Q77" s="58"/>
-      <c r="R77" s="58"/>
-      <c r="S77" s="58"/>
-      <c r="T77" s="58"/>
-      <c r="U77" s="58"/>
-      <c r="V77" s="58"/>
-      <c r="W77" s="58"/>
-      <c r="X77" s="58"/>
-      <c r="Y77" s="58"/>
-      <c r="Z77" s="58"/>
-      <c r="AA77" s="58"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="45"/>
+      <c r="L77" s="45"/>
+      <c r="M77" s="45"/>
+      <c r="N77" s="45"/>
+      <c r="O77" s="45"/>
+      <c r="P77" s="45"/>
+      <c r="Q77" s="45"/>
+      <c r="R77" s="45"/>
+      <c r="S77" s="45"/>
+      <c r="T77" s="45"/>
+      <c r="U77" s="45"/>
+      <c r="V77" s="45"/>
+      <c r="W77" s="45"/>
+      <c r="X77" s="45"/>
+      <c r="Y77" s="45"/>
+      <c r="Z77" s="45"/>
+      <c r="AA77" s="45"/>
     </row>
     <row r="78" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="55">
+      <c r="A78" s="42">
         <v>76</v>
       </c>
-      <c r="B78" s="58"/>
-      <c r="C78" s="58" t="s">
+      <c r="B78" s="45"/>
+      <c r="C78" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="D78" s="58"/>
-      <c r="E78" s="57" t="s">
+      <c r="D78" s="45"/>
+      <c r="E78" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F78" s="58"/>
-      <c r="G78" s="58"/>
-      <c r="H78" s="58"/>
-      <c r="I78" s="58"/>
-      <c r="J78" s="58"/>
-      <c r="K78" s="58"/>
-      <c r="L78" s="58"/>
-      <c r="M78" s="58"/>
-      <c r="N78" s="58"/>
-      <c r="O78" s="58"/>
-      <c r="P78" s="58"/>
-      <c r="Q78" s="58"/>
-      <c r="R78" s="58"/>
-      <c r="S78" s="58"/>
-      <c r="T78" s="58"/>
-      <c r="U78" s="58"/>
-      <c r="V78" s="58"/>
-      <c r="W78" s="58"/>
-      <c r="X78" s="58"/>
-      <c r="Y78" s="58"/>
-      <c r="Z78" s="58"/>
-      <c r="AA78" s="58"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="45"/>
+      <c r="H78" s="45"/>
+      <c r="I78" s="45"/>
+      <c r="J78" s="45"/>
+      <c r="K78" s="45"/>
+      <c r="L78" s="45"/>
+      <c r="M78" s="45"/>
+      <c r="N78" s="45"/>
+      <c r="O78" s="45"/>
+      <c r="P78" s="45"/>
+      <c r="Q78" s="45"/>
+      <c r="R78" s="45"/>
+      <c r="S78" s="45"/>
+      <c r="T78" s="45"/>
+      <c r="U78" s="45"/>
+      <c r="V78" s="45"/>
+      <c r="W78" s="45"/>
+      <c r="X78" s="45"/>
+      <c r="Y78" s="45"/>
+      <c r="Z78" s="45"/>
+      <c r="AA78" s="45"/>
     </row>
     <row r="79" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="55">
+      <c r="A79" s="42">
         <v>77</v>
       </c>
-      <c r="B79" s="58"/>
-      <c r="C79" s="58" t="s">
+      <c r="B79" s="45"/>
+      <c r="C79" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="D79" s="58"/>
-      <c r="E79" s="57" t="s">
+      <c r="D79" s="45"/>
+      <c r="E79" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F79" s="58"/>
-      <c r="G79" s="58"/>
-      <c r="H79" s="58"/>
-      <c r="I79" s="58"/>
-      <c r="J79" s="58"/>
-      <c r="K79" s="58"/>
-      <c r="L79" s="58"/>
-      <c r="M79" s="58"/>
-      <c r="N79" s="58"/>
-      <c r="O79" s="58"/>
-      <c r="P79" s="58"/>
-      <c r="Q79" s="58"/>
-      <c r="R79" s="58"/>
-      <c r="S79" s="58"/>
-      <c r="T79" s="58"/>
-      <c r="U79" s="58"/>
-      <c r="V79" s="58"/>
-      <c r="W79" s="58"/>
-      <c r="X79" s="58"/>
-      <c r="Y79" s="58"/>
-      <c r="Z79" s="58"/>
-      <c r="AA79" s="58"/>
+      <c r="F79" s="45"/>
+      <c r="G79" s="45"/>
+      <c r="H79" s="45"/>
+      <c r="I79" s="45"/>
+      <c r="J79" s="45"/>
+      <c r="K79" s="45"/>
+      <c r="L79" s="45"/>
+      <c r="M79" s="45"/>
+      <c r="N79" s="45"/>
+      <c r="O79" s="45"/>
+      <c r="P79" s="45"/>
+      <c r="Q79" s="45"/>
+      <c r="R79" s="45"/>
+      <c r="S79" s="45"/>
+      <c r="T79" s="45"/>
+      <c r="U79" s="45"/>
+      <c r="V79" s="45"/>
+      <c r="W79" s="45"/>
+      <c r="X79" s="45"/>
+      <c r="Y79" s="45"/>
+      <c r="Z79" s="45"/>
+      <c r="AA79" s="45"/>
     </row>
     <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="55"/>
-      <c r="B80" s="58"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
-      <c r="F80" s="58"/>
-      <c r="G80" s="58"/>
-      <c r="H80" s="58"/>
-      <c r="I80" s="58"/>
-      <c r="J80" s="58"/>
-      <c r="K80" s="58"/>
-      <c r="L80" s="58"/>
-      <c r="M80" s="58"/>
-      <c r="N80" s="58"/>
-      <c r="O80" s="58"/>
-      <c r="P80" s="58"/>
-      <c r="Q80" s="58"/>
-      <c r="R80" s="58"/>
-      <c r="S80" s="58"/>
-      <c r="T80" s="58"/>
-      <c r="U80" s="58"/>
-      <c r="V80" s="58"/>
-      <c r="W80" s="58"/>
-      <c r="X80" s="58"/>
-      <c r="Y80" s="58"/>
-      <c r="Z80" s="58"/>
-      <c r="AA80" s="58"/>
+      <c r="A80" s="42"/>
+      <c r="B80" s="45"/>
+      <c r="C80" s="45"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+      <c r="J80" s="45"/>
+      <c r="K80" s="45"/>
+      <c r="L80" s="45"/>
+      <c r="M80" s="45"/>
+      <c r="N80" s="45"/>
+      <c r="O80" s="45"/>
+      <c r="P80" s="45"/>
+      <c r="Q80" s="45"/>
+      <c r="R80" s="45"/>
+      <c r="S80" s="45"/>
+      <c r="T80" s="45"/>
+      <c r="U80" s="45"/>
+      <c r="V80" s="45"/>
+      <c r="W80" s="45"/>
+      <c r="X80" s="45"/>
+      <c r="Y80" s="45"/>
+      <c r="Z80" s="45"/>
+      <c r="AA80" s="45"/>
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="55"/>
-      <c r="B81" s="58"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="58"/>
-      <c r="G81" s="58"/>
-      <c r="H81" s="58"/>
-      <c r="I81" s="58"/>
-      <c r="J81" s="58"/>
-      <c r="K81" s="58"/>
-      <c r="L81" s="58"/>
-      <c r="M81" s="58"/>
-      <c r="N81" s="58"/>
-      <c r="O81" s="58"/>
-      <c r="P81" s="58"/>
-      <c r="Q81" s="58"/>
-      <c r="R81" s="58"/>
-      <c r="S81" s="58"/>
-      <c r="T81" s="58"/>
-      <c r="U81" s="58"/>
-      <c r="V81" s="58"/>
-      <c r="W81" s="58"/>
-      <c r="X81" s="58"/>
-      <c r="Y81" s="58"/>
-      <c r="Z81" s="58"/>
-      <c r="AA81" s="58"/>
+      <c r="A81" s="42"/>
+      <c r="B81" s="45"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="45"/>
+      <c r="H81" s="45"/>
+      <c r="I81" s="45"/>
+      <c r="J81" s="45"/>
+      <c r="K81" s="45"/>
+      <c r="L81" s="45"/>
+      <c r="M81" s="45"/>
+      <c r="N81" s="45"/>
+      <c r="O81" s="45"/>
+      <c r="P81" s="45"/>
+      <c r="Q81" s="45"/>
+      <c r="R81" s="45"/>
+      <c r="S81" s="45"/>
+      <c r="T81" s="45"/>
+      <c r="U81" s="45"/>
+      <c r="V81" s="45"/>
+      <c r="W81" s="45"/>
+      <c r="X81" s="45"/>
+      <c r="Y81" s="45"/>
+      <c r="Z81" s="45"/>
+      <c r="AA81" s="45"/>
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="58"/>
-      <c r="B82" s="58"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="58"/>
-      <c r="G82" s="58"/>
-      <c r="H82" s="58"/>
-      <c r="I82" s="58"/>
-      <c r="J82" s="58"/>
-      <c r="K82" s="58"/>
-      <c r="L82" s="58"/>
-      <c r="M82" s="58"/>
-      <c r="N82" s="58"/>
-      <c r="O82" s="58"/>
-      <c r="P82" s="58"/>
-      <c r="Q82" s="58"/>
-      <c r="R82" s="58"/>
-      <c r="S82" s="58"/>
-      <c r="T82" s="58"/>
-      <c r="U82" s="58"/>
-      <c r="V82" s="58"/>
-      <c r="W82" s="58"/>
-      <c r="X82" s="58"/>
-      <c r="Y82" s="58"/>
-      <c r="Z82" s="58"/>
-      <c r="AA82" s="58"/>
+      <c r="A82" s="45"/>
+      <c r="B82" s="45"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+      <c r="J82" s="45"/>
+      <c r="K82" s="45"/>
+      <c r="L82" s="45"/>
+      <c r="M82" s="45"/>
+      <c r="N82" s="45"/>
+      <c r="O82" s="45"/>
+      <c r="P82" s="45"/>
+      <c r="Q82" s="45"/>
+      <c r="R82" s="45"/>
+      <c r="S82" s="45"/>
+      <c r="T82" s="45"/>
+      <c r="U82" s="45"/>
+      <c r="V82" s="45"/>
+      <c r="W82" s="45"/>
+      <c r="X82" s="45"/>
+      <c r="Y82" s="45"/>
+      <c r="Z82" s="45"/>
+      <c r="AA82" s="45"/>
     </row>
     <row r="83" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="58"/>
-      <c r="B83" s="58"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
-      <c r="H83" s="58"/>
-      <c r="I83" s="58"/>
-      <c r="J83" s="58"/>
-      <c r="K83" s="58"/>
-      <c r="L83" s="58"/>
-      <c r="M83" s="58"/>
-      <c r="N83" s="58"/>
-      <c r="O83" s="58"/>
-      <c r="P83" s="58"/>
-      <c r="Q83" s="58"/>
-      <c r="R83" s="58"/>
-      <c r="S83" s="58"/>
-      <c r="T83" s="58"/>
-      <c r="U83" s="58"/>
-      <c r="V83" s="58"/>
-      <c r="W83" s="58"/>
-      <c r="X83" s="58"/>
-      <c r="Y83" s="58"/>
-      <c r="Z83" s="58"/>
-      <c r="AA83" s="58"/>
+      <c r="A83" s="45"/>
+      <c r="B83" s="45"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="45"/>
+      <c r="I83" s="45"/>
+      <c r="J83" s="45"/>
+      <c r="K83" s="45"/>
+      <c r="L83" s="45"/>
+      <c r="M83" s="45"/>
+      <c r="N83" s="45"/>
+      <c r="O83" s="45"/>
+      <c r="P83" s="45"/>
+      <c r="Q83" s="45"/>
+      <c r="R83" s="45"/>
+      <c r="S83" s="45"/>
+      <c r="T83" s="45"/>
+      <c r="U83" s="45"/>
+      <c r="V83" s="45"/>
+      <c r="W83" s="45"/>
+      <c r="X83" s="45"/>
+      <c r="Y83" s="45"/>
+      <c r="Z83" s="45"/>
+      <c r="AA83" s="45"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="58"/>
-      <c r="B84" s="58"/>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
-      <c r="I84" s="58"/>
-      <c r="J84" s="58"/>
-      <c r="K84" s="58"/>
-      <c r="L84" s="58"/>
-      <c r="M84" s="58"/>
-      <c r="N84" s="58"/>
-      <c r="O84" s="58"/>
-      <c r="P84" s="58"/>
-      <c r="Q84" s="58"/>
-      <c r="R84" s="58"/>
-      <c r="S84" s="58"/>
-      <c r="T84" s="58"/>
-      <c r="U84" s="58"/>
-      <c r="V84" s="58"/>
-      <c r="W84" s="58"/>
-      <c r="X84" s="58"/>
-      <c r="Y84" s="58"/>
-      <c r="Z84" s="58"/>
-      <c r="AA84" s="58"/>
+      <c r="A84" s="45"/>
+      <c r="B84" s="45"/>
+      <c r="C84" s="45"/>
+      <c r="D84" s="45"/>
+      <c r="E84" s="45"/>
+      <c r="F84" s="45"/>
+      <c r="G84" s="45"/>
+      <c r="H84" s="45"/>
+      <c r="I84" s="45"/>
+      <c r="J84" s="45"/>
+      <c r="K84" s="45"/>
+      <c r="L84" s="45"/>
+      <c r="M84" s="45"/>
+      <c r="N84" s="45"/>
+      <c r="O84" s="45"/>
+      <c r="P84" s="45"/>
+      <c r="Q84" s="45"/>
+      <c r="R84" s="45"/>
+      <c r="S84" s="45"/>
+      <c r="T84" s="45"/>
+      <c r="U84" s="45"/>
+      <c r="V84" s="45"/>
+      <c r="W84" s="45"/>
+      <c r="X84" s="45"/>
+      <c r="Y84" s="45"/>
+      <c r="Z84" s="45"/>
+      <c r="AA84" s="45"/>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="58"/>
-      <c r="B85" s="58"/>
-      <c r="C85" s="58"/>
-      <c r="D85" s="58"/>
-      <c r="E85" s="58"/>
-      <c r="F85" s="58"/>
-      <c r="G85" s="58"/>
-      <c r="H85" s="58"/>
-      <c r="I85" s="58"/>
-      <c r="J85" s="58"/>
-      <c r="K85" s="58"/>
-      <c r="L85" s="58"/>
-      <c r="M85" s="58"/>
-      <c r="N85" s="58"/>
-      <c r="O85" s="58"/>
-      <c r="P85" s="58"/>
-      <c r="Q85" s="58"/>
-      <c r="R85" s="58"/>
-      <c r="S85" s="58"/>
-      <c r="T85" s="58"/>
-      <c r="U85" s="58"/>
-      <c r="V85" s="58"/>
-      <c r="W85" s="58"/>
-      <c r="X85" s="58"/>
-      <c r="Y85" s="58"/>
-      <c r="Z85" s="58"/>
-      <c r="AA85" s="58"/>
+      <c r="A85" s="45"/>
+      <c r="B85" s="45"/>
+      <c r="C85" s="45"/>
+      <c r="D85" s="45"/>
+      <c r="E85" s="45"/>
+      <c r="F85" s="45"/>
+      <c r="G85" s="45"/>
+      <c r="H85" s="45"/>
+      <c r="I85" s="45"/>
+      <c r="J85" s="45"/>
+      <c r="K85" s="45"/>
+      <c r="L85" s="45"/>
+      <c r="M85" s="45"/>
+      <c r="N85" s="45"/>
+      <c r="O85" s="45"/>
+      <c r="P85" s="45"/>
+      <c r="Q85" s="45"/>
+      <c r="R85" s="45"/>
+      <c r="S85" s="45"/>
+      <c r="T85" s="45"/>
+      <c r="U85" s="45"/>
+      <c r="V85" s="45"/>
+      <c r="W85" s="45"/>
+      <c r="X85" s="45"/>
+      <c r="Y85" s="45"/>
+      <c r="Z85" s="45"/>
+      <c r="AA85" s="45"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="58"/>
-      <c r="B86" s="58"/>
-      <c r="C86" s="58"/>
-      <c r="D86" s="58"/>
-      <c r="E86" s="58"/>
-      <c r="F86" s="58"/>
-      <c r="G86" s="58"/>
-      <c r="H86" s="58"/>
-      <c r="I86" s="58"/>
-      <c r="J86" s="58"/>
-      <c r="K86" s="58"/>
-      <c r="L86" s="58"/>
-      <c r="M86" s="58"/>
-      <c r="N86" s="58"/>
-      <c r="O86" s="58"/>
-      <c r="P86" s="58"/>
-      <c r="Q86" s="58"/>
-      <c r="R86" s="58"/>
-      <c r="S86" s="58"/>
-      <c r="T86" s="58"/>
-      <c r="U86" s="58"/>
-      <c r="V86" s="58"/>
-      <c r="W86" s="58"/>
-      <c r="X86" s="58"/>
-      <c r="Y86" s="58"/>
-      <c r="Z86" s="58"/>
-      <c r="AA86" s="58"/>
+      <c r="A86" s="45"/>
+      <c r="B86" s="45"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="45"/>
+      <c r="I86" s="45"/>
+      <c r="J86" s="45"/>
+      <c r="K86" s="45"/>
+      <c r="L86" s="45"/>
+      <c r="M86" s="45"/>
+      <c r="N86" s="45"/>
+      <c r="O86" s="45"/>
+      <c r="P86" s="45"/>
+      <c r="Q86" s="45"/>
+      <c r="R86" s="45"/>
+      <c r="S86" s="45"/>
+      <c r="T86" s="45"/>
+      <c r="U86" s="45"/>
+      <c r="V86" s="45"/>
+      <c r="W86" s="45"/>
+      <c r="X86" s="45"/>
+      <c r="Y86" s="45"/>
+      <c r="Z86" s="45"/>
+      <c r="AA86" s="45"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="58"/>
-      <c r="B87" s="58"/>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
-      <c r="I87" s="58"/>
-      <c r="J87" s="58"/>
-      <c r="K87" s="58"/>
-      <c r="L87" s="58"/>
-      <c r="M87" s="58"/>
-      <c r="N87" s="58"/>
-      <c r="O87" s="58"/>
-      <c r="P87" s="58"/>
-      <c r="Q87" s="58"/>
-      <c r="R87" s="58"/>
-      <c r="S87" s="58"/>
-      <c r="T87" s="58"/>
-      <c r="U87" s="58"/>
-      <c r="V87" s="58"/>
-      <c r="W87" s="58"/>
-      <c r="X87" s="58"/>
-      <c r="Y87" s="58"/>
-      <c r="Z87" s="58"/>
-      <c r="AA87" s="58"/>
+      <c r="A87" s="45"/>
+      <c r="B87" s="45"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="45"/>
+      <c r="J87" s="45"/>
+      <c r="K87" s="45"/>
+      <c r="L87" s="45"/>
+      <c r="M87" s="45"/>
+      <c r="N87" s="45"/>
+      <c r="O87" s="45"/>
+      <c r="P87" s="45"/>
+      <c r="Q87" s="45"/>
+      <c r="R87" s="45"/>
+      <c r="S87" s="45"/>
+      <c r="T87" s="45"/>
+      <c r="U87" s="45"/>
+      <c r="V87" s="45"/>
+      <c r="W87" s="45"/>
+      <c r="X87" s="45"/>
+      <c r="Y87" s="45"/>
+      <c r="Z87" s="45"/>
+      <c r="AA87" s="45"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="58"/>
-      <c r="B88" s="58"/>
-      <c r="C88" s="58"/>
-      <c r="D88" s="58"/>
-      <c r="E88" s="58"/>
-      <c r="F88" s="58"/>
-      <c r="G88" s="58"/>
-      <c r="H88" s="58"/>
-      <c r="I88" s="58"/>
-      <c r="J88" s="58"/>
-      <c r="K88" s="58"/>
-      <c r="L88" s="58"/>
-      <c r="M88" s="58"/>
-      <c r="N88" s="58"/>
-      <c r="O88" s="58"/>
-      <c r="P88" s="58"/>
-      <c r="Q88" s="58"/>
-      <c r="R88" s="58"/>
-      <c r="S88" s="58"/>
-      <c r="T88" s="58"/>
-      <c r="U88" s="58"/>
-      <c r="V88" s="58"/>
-      <c r="W88" s="58"/>
-      <c r="X88" s="58"/>
-      <c r="Y88" s="58"/>
-      <c r="Z88" s="58"/>
-      <c r="AA88" s="58"/>
+      <c r="A88" s="45"/>
+      <c r="B88" s="45"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45"/>
+      <c r="G88" s="45"/>
+      <c r="H88" s="45"/>
+      <c r="I88" s="45"/>
+      <c r="J88" s="45"/>
+      <c r="K88" s="45"/>
+      <c r="L88" s="45"/>
+      <c r="M88" s="45"/>
+      <c r="N88" s="45"/>
+      <c r="O88" s="45"/>
+      <c r="P88" s="45"/>
+      <c r="Q88" s="45"/>
+      <c r="R88" s="45"/>
+      <c r="S88" s="45"/>
+      <c r="T88" s="45"/>
+      <c r="U88" s="45"/>
+      <c r="V88" s="45"/>
+      <c r="W88" s="45"/>
+      <c r="X88" s="45"/>
+      <c r="Y88" s="45"/>
+      <c r="Z88" s="45"/>
+      <c r="AA88" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4759,8 +4758,8 @@
   </sheetPr>
   <dimension ref="A1:AK1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4772,91 +4771,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="49" t="s">
+      <c r="L1" s="59"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="44"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="43" t="s">
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="49" t="s">
+      <c r="R1" s="59"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="44"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="43" t="s">
+      <c r="U1" s="59"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="49" t="s">
+      <c r="X1" s="59"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="43" t="s">
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="49" t="s">
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
+      <c r="AF1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="43" t="s">
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="60"/>
+      <c r="AI1" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="45"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="60"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="47"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -4939,20 +4938,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="48"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -34849,16 +34848,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -34867,6 +34856,16 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>